<commit_message>
updated end of day for all 4ml horz runs of beads
</commit_message>
<xml_diff>
--- a/Development/IFCB_vehicles/VehicleLabExperimentFiles.xlsx
+++ b/Development/IFCB_vehicles/VehicleLabExperimentFiles.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\ifcb-analysis\IFCB_vehicles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\ifcb-analysis\Development\IFCB_vehicles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="61">
   <si>
     <t>Filename</t>
   </si>
@@ -193,6 +193,21 @@
   </si>
   <si>
     <t>D20151103T200533</t>
+  </si>
+  <si>
+    <t>D20151103T202347</t>
+  </si>
+  <si>
+    <t>D20151103T204202</t>
+  </si>
+  <si>
+    <t>D20151103T210016</t>
+  </si>
+  <si>
+    <t>D20151103T211831</t>
+  </si>
+  <si>
+    <t>D20151103T214021</t>
   </si>
 </sst>
 </file>
@@ -807,10 +822,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1389,6 +1404,133 @@
         <v>41</v>
       </c>
     </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19">
+        <v>560.4</v>
+      </c>
+      <c r="E19">
+        <v>3.3262999999999998</v>
+      </c>
+      <c r="F19">
+        <v>958</v>
+      </c>
+      <c r="G19">
+        <v>144.69999999999999</v>
+      </c>
+      <c r="H19">
+        <v>1864</v>
+      </c>
+      <c r="I19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20">
+        <v>575.70000000000005</v>
+      </c>
+      <c r="E20">
+        <v>3.3142999999999998</v>
+      </c>
+      <c r="F20">
+        <v>958</v>
+      </c>
+      <c r="G20">
+        <v>148.07</v>
+      </c>
+      <c r="H20">
+        <v>1908</v>
+      </c>
+      <c r="I20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21">
+        <v>599.29999999999995</v>
+      </c>
+      <c r="E21">
+        <v>3.2921</v>
+      </c>
+      <c r="F21">
+        <v>958</v>
+      </c>
+      <c r="G21">
+        <v>153.1</v>
+      </c>
+      <c r="H21">
+        <v>1973</v>
+      </c>
+      <c r="I21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22">
+        <v>557.6</v>
+      </c>
+      <c r="E22">
+        <v>3.3338000000000001</v>
+      </c>
+      <c r="F22">
+        <v>958</v>
+      </c>
+      <c r="G22">
+        <v>143.5</v>
+      </c>
+      <c r="H22">
+        <v>1859</v>
+      </c>
+      <c r="I22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated files with cell conc. made new beads because didnt' go back to vert runs in time before solution got junk in it
</commit_message>
<xml_diff>
--- a/Development/IFCB_vehicles/VehicleLabExperimentFiles.xlsx
+++ b/Development/IFCB_vehicles/VehicleLabExperimentFiles.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="90">
   <si>
     <t>Filename</t>
   </si>
@@ -111,15 +111,9 @@
     <t>D20151103T145610</t>
   </si>
   <si>
-    <t>D20151103T151633</t>
-  </si>
-  <si>
     <t>D20151103T152713</t>
   </si>
   <si>
-    <t>realize incorrectly running 2ml when want to run 5ml</t>
-  </si>
-  <si>
     <t>D20151103T154933</t>
   </si>
   <si>
@@ -144,12 +138,6 @@
     <t>numtriggers</t>
   </si>
   <si>
-    <t>D20151103T165631</t>
-  </si>
-  <si>
-    <t>sampled ended early because concentration consistent enough to move on to next stage: horz 5ml runs</t>
-  </si>
-  <si>
     <t>9um beads, use all signals</t>
   </si>
   <si>
@@ -171,9 +159,6 @@
     <t>D20151103T181654</t>
   </si>
   <si>
-    <t>5*</t>
-  </si>
-  <si>
     <t>2*</t>
   </si>
   <si>
@@ -208,6 +193,108 @@
   </si>
   <si>
     <t>D20151103T214021</t>
+  </si>
+  <si>
+    <t>D20151103T215521</t>
+  </si>
+  <si>
+    <t>D20151103T220931</t>
+  </si>
+  <si>
+    <t>D20151103T222341</t>
+  </si>
+  <si>
+    <t>D20151103T223750</t>
+  </si>
+  <si>
+    <t>D20151103T225200</t>
+  </si>
+  <si>
+    <t>D20151103T230609</t>
+  </si>
+  <si>
+    <t>D20151103T232019</t>
+  </si>
+  <si>
+    <t>D20151104T145502</t>
+  </si>
+  <si>
+    <t>D20151104T150507</t>
+  </si>
+  <si>
+    <t>D20151104T151512</t>
+  </si>
+  <si>
+    <t>D20151104T152517</t>
+  </si>
+  <si>
+    <t>D20151104T154347</t>
+  </si>
+  <si>
+    <t>**first vert run after horz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D20151104T162848 </t>
+  </si>
+  <si>
+    <t>*5</t>
+  </si>
+  <si>
+    <t>run stopped short, beads solution is dirty so won't work for analysis, make fresh beads and start over</t>
+  </si>
+  <si>
+    <t>D20151104T171015</t>
+  </si>
+  <si>
+    <t>D20151104T173233</t>
+  </si>
+  <si>
+    <t>D20151104T160619</t>
+  </si>
+  <si>
+    <t>fresh bead in FSW just made</t>
+  </si>
+  <si>
+    <t>nice clean soln no junk seen, back to good roi pos, laser off so high ypos pmtB signals no good.</t>
+  </si>
+  <si>
+    <t>D20151104T175453</t>
+  </si>
+  <si>
+    <t>pull plug to stop from sampling air because autostarted</t>
+  </si>
+  <si>
+    <t>D20151104T182649</t>
+  </si>
+  <si>
+    <t>roi position back to okay, some junk in but not as much?</t>
+  </si>
+  <si>
+    <t>still just beads, no junk, some out of focus a bit, pos good</t>
+  </si>
+  <si>
+    <t>a few small pieces of junk seen</t>
+  </si>
+  <si>
+    <t>not much junk at all this time</t>
+  </si>
+  <si>
+    <t>next day, junk def in sample, sat overnight stuff settled in? also dumped some of waste cup to avoid overflow</t>
+  </si>
+  <si>
+    <t>junk with beads</t>
+  </si>
+  <si>
+    <t>D20151104T184948</t>
+  </si>
+  <si>
+    <t>D20151104T191208</t>
+  </si>
+  <si>
+    <t>pos good, no junk, pos a little higher?</t>
+  </si>
+  <si>
+    <t>pos good, no junk, conc slightly lower</t>
   </si>
 </sst>
 </file>
@@ -223,12 +310,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -243,11 +336,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -822,10 +917,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,16 +950,16 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="I1" t="s">
         <v>6</v>
@@ -877,7 +973,7 @@
         <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -904,7 +1000,7 @@
         <v>24</v>
       </c>
       <c r="K2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -936,42 +1032,39 @@
         <v>23</v>
       </c>
       <c r="J3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
-      <c r="B4" t="s">
-        <v>48</v>
+      <c r="B4">
+        <v>5</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
       <c r="D4">
-        <v>583</v>
+        <v>633</v>
       </c>
       <c r="E4">
-        <v>1.6419999999999999</v>
+        <v>4.1097999999999999</v>
       </c>
       <c r="F4">
-        <v>478</v>
+        <v>1198</v>
       </c>
       <c r="G4">
-        <v>68.44</v>
+        <v>211.6</v>
       </c>
       <c r="H4">
-        <v>958</v>
+        <v>2605</v>
       </c>
       <c r="I4" t="s">
         <v>23</v>
       </c>
       <c r="J4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -985,30 +1078,30 @@
         <v>5</v>
       </c>
       <c r="D5">
-        <v>633</v>
+        <v>637.70000000000005</v>
       </c>
       <c r="E5">
-        <v>4.1097999999999999</v>
+        <v>4.0865</v>
       </c>
       <c r="F5">
-        <v>1198</v>
+        <v>1198.04</v>
       </c>
       <c r="G5">
-        <v>211.6</v>
+        <v>202.27199999999999</v>
       </c>
       <c r="H5">
-        <v>2605</v>
+        <v>2606</v>
       </c>
       <c r="I5" t="s">
         <v>23</v>
       </c>
       <c r="J5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -1017,30 +1110,30 @@
         <v>5</v>
       </c>
       <c r="D6">
-        <v>637.70000000000005</v>
+        <v>636.6</v>
       </c>
       <c r="E6">
-        <v>4.0865</v>
+        <v>4.0888</v>
       </c>
       <c r="F6">
-        <v>1198.04</v>
+        <v>1198</v>
       </c>
       <c r="G6">
-        <v>202.27199999999999</v>
+        <v>204.11</v>
       </c>
       <c r="H6">
-        <v>2606</v>
+        <v>2603</v>
       </c>
       <c r="I6" t="s">
         <v>23</v>
       </c>
       <c r="J6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7">
         <v>5</v>
@@ -1049,94 +1142,94 @@
         <v>5</v>
       </c>
       <c r="D7">
-        <v>636.6</v>
+        <v>635.6</v>
       </c>
       <c r="E7">
-        <v>4.0888</v>
+        <v>4.0873999999999997</v>
       </c>
       <c r="F7">
         <v>1198</v>
       </c>
       <c r="G7">
-        <v>204.11</v>
+        <v>201.6</v>
       </c>
       <c r="H7">
-        <v>2603</v>
+        <v>2598</v>
       </c>
       <c r="I7" t="s">
         <v>23</v>
       </c>
       <c r="J7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B8">
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D8">
-        <v>635.6</v>
+        <v>580</v>
       </c>
       <c r="E8">
-        <v>4.0873999999999997</v>
+        <v>4.1439000000000004</v>
       </c>
       <c r="F8">
         <v>1198</v>
       </c>
       <c r="G8">
-        <v>201.6</v>
+        <v>187</v>
       </c>
       <c r="H8">
-        <v>2598</v>
+        <v>2403</v>
       </c>
       <c r="I8" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="J8" t="s">
-        <v>34</v>
+        <v>42</v>
+      </c>
+      <c r="K8" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>39</v>
       </c>
-      <c r="B9" t="s">
-        <v>48</v>
+      <c r="B9">
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D9">
-        <v>600</v>
+        <v>580.1</v>
       </c>
       <c r="E9">
-        <v>1.1843999999999999</v>
+        <v>4.1440999999999999</v>
       </c>
       <c r="F9">
-        <v>351.2</v>
+        <v>1198</v>
       </c>
       <c r="G9">
-        <v>56.13</v>
+        <v>188.78</v>
       </c>
       <c r="H9">
-        <v>711</v>
+        <v>2404</v>
       </c>
       <c r="I9" t="s">
-        <v>40</v>
-      </c>
-      <c r="J9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B10">
         <v>5</v>
@@ -1145,28 +1238,22 @@
         <v>10</v>
       </c>
       <c r="D10">
-        <v>580</v>
+        <v>591.6</v>
       </c>
       <c r="E10">
-        <v>4.1439000000000004</v>
+        <v>4.1295999999999999</v>
       </c>
       <c r="F10">
         <v>1198</v>
       </c>
       <c r="G10">
-        <v>187</v>
+        <v>190.1</v>
       </c>
       <c r="H10">
-        <v>2403</v>
+        <v>2443</v>
       </c>
       <c r="I10" t="s">
-        <v>45</v>
-      </c>
-      <c r="J10" t="s">
-        <v>46</v>
-      </c>
-      <c r="K10" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1180,27 +1267,27 @@
         <v>10</v>
       </c>
       <c r="D11">
-        <v>580.1</v>
+        <v>565.70000000000005</v>
       </c>
       <c r="E11">
-        <v>4.1440999999999999</v>
+        <v>4.1664000000000003</v>
       </c>
       <c r="F11">
         <v>1198</v>
       </c>
       <c r="G11">
-        <v>188.78</v>
+        <v>183.6</v>
       </c>
       <c r="H11">
-        <v>2404</v>
+        <v>2357</v>
       </c>
       <c r="I11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B12">
         <v>5</v>
@@ -1209,27 +1296,27 @@
         <v>10</v>
       </c>
       <c r="D12">
-        <v>591.6</v>
+        <v>543.4</v>
       </c>
       <c r="E12">
-        <v>4.1295999999999999</v>
+        <v>4.2340999999999998</v>
       </c>
       <c r="F12">
         <v>1198</v>
       </c>
       <c r="G12">
-        <v>190.1</v>
+        <v>181.79</v>
       </c>
       <c r="H12">
-        <v>2443</v>
+        <v>2301</v>
       </c>
       <c r="I12" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B13">
         <v>5</v>
@@ -1238,85 +1325,88 @@
         <v>10</v>
       </c>
       <c r="D13">
-        <v>565.70000000000005</v>
+        <v>578.29999999999995</v>
       </c>
       <c r="E13">
-        <v>4.1664000000000003</v>
+        <v>4.1193</v>
       </c>
       <c r="F13">
         <v>1198</v>
       </c>
       <c r="G13">
-        <v>183.6</v>
+        <v>192.3</v>
       </c>
       <c r="H13">
-        <v>2357</v>
+        <v>2382</v>
       </c>
       <c r="I13" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14" t="s">
         <v>10</v>
       </c>
       <c r="D14">
-        <v>543.4</v>
+        <v>599.23</v>
       </c>
       <c r="E14">
-        <v>4.2340999999999998</v>
+        <v>3.2942</v>
       </c>
       <c r="F14">
-        <v>1198</v>
+        <v>958</v>
       </c>
       <c r="G14">
-        <v>181.79</v>
+        <v>153.74</v>
       </c>
       <c r="H14">
-        <v>2301</v>
+        <v>1974</v>
       </c>
       <c r="I14" t="s">
-        <v>41</v>
+        <v>48</v>
+      </c>
+      <c r="J14" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B15">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C15" t="s">
         <v>10</v>
       </c>
       <c r="D15">
-        <v>578.29999999999995</v>
+        <v>567.57000000000005</v>
       </c>
       <c r="E15">
-        <v>4.1193</v>
+        <v>3.3740000000000001</v>
       </c>
       <c r="F15">
-        <v>1198</v>
+        <v>958</v>
       </c>
       <c r="G15">
-        <v>192.3</v>
+        <v>148.19999999999999</v>
       </c>
       <c r="H15">
-        <v>2382</v>
+        <v>1915</v>
       </c>
       <c r="I15" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -1325,30 +1415,27 @@
         <v>10</v>
       </c>
       <c r="D16">
-        <v>599.23</v>
+        <v>570</v>
       </c>
       <c r="E16">
-        <v>3.2942</v>
+        <v>3.3136999999999999</v>
       </c>
       <c r="F16">
         <v>958</v>
       </c>
       <c r="G16">
-        <v>153.74</v>
+        <v>146.44999999999999</v>
       </c>
       <c r="H16">
-        <v>1974</v>
+        <v>1889</v>
       </c>
       <c r="I16" t="s">
-        <v>53</v>
-      </c>
-      <c r="J16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B17">
         <v>4</v>
@@ -1357,27 +1444,27 @@
         <v>10</v>
       </c>
       <c r="D17">
-        <v>567.57000000000005</v>
+        <v>560.4</v>
       </c>
       <c r="E17">
-        <v>3.3740000000000001</v>
+        <v>3.3262999999999998</v>
       </c>
       <c r="F17">
         <v>958</v>
       </c>
       <c r="G17">
-        <v>148.19999999999999</v>
+        <v>144.69999999999999</v>
       </c>
       <c r="H17">
-        <v>1915</v>
+        <v>1864</v>
       </c>
       <c r="I17" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B18">
         <v>4</v>
@@ -1386,27 +1473,27 @@
         <v>10</v>
       </c>
       <c r="D18">
-        <v>570</v>
+        <v>575.70000000000005</v>
       </c>
       <c r="E18">
-        <v>3.3136999999999999</v>
+        <v>3.3142999999999998</v>
       </c>
       <c r="F18">
         <v>958</v>
       </c>
       <c r="G18">
-        <v>146.44999999999999</v>
+        <v>148.07</v>
       </c>
       <c r="H18">
-        <v>1889</v>
+        <v>1908</v>
       </c>
       <c r="I18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B19">
         <v>4</v>
@@ -1415,27 +1502,27 @@
         <v>10</v>
       </c>
       <c r="D19">
-        <v>560.4</v>
+        <v>599.29999999999995</v>
       </c>
       <c r="E19">
-        <v>3.3262999999999998</v>
+        <v>3.2921</v>
       </c>
       <c r="F19">
         <v>958</v>
       </c>
       <c r="G19">
-        <v>144.69999999999999</v>
+        <v>153.1</v>
       </c>
       <c r="H19">
-        <v>1864</v>
+        <v>1973</v>
       </c>
       <c r="I19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B20">
         <v>4</v>
@@ -1444,91 +1531,637 @@
         <v>10</v>
       </c>
       <c r="D20">
-        <v>575.70000000000005</v>
+        <v>557.6</v>
       </c>
       <c r="E20">
-        <v>3.3142999999999998</v>
+        <v>3.3338000000000001</v>
       </c>
       <c r="F20">
         <v>958</v>
       </c>
       <c r="G20">
-        <v>148.07</v>
+        <v>143.5</v>
       </c>
       <c r="H20">
-        <v>1908</v>
+        <v>1859</v>
       </c>
       <c r="I20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B21">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C21" t="s">
         <v>10</v>
       </c>
       <c r="D21">
-        <v>599.29999999999995</v>
+        <v>587.20000000000005</v>
       </c>
       <c r="E21">
-        <v>3.2921</v>
+        <v>2.4521999999999999</v>
       </c>
       <c r="F21">
-        <v>958</v>
+        <v>718</v>
       </c>
       <c r="G21">
-        <v>153.1</v>
+        <v>113.27</v>
       </c>
       <c r="H21">
-        <v>1973</v>
+        <v>1440</v>
       </c>
       <c r="I21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="J21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B22">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C22" t="s">
         <v>10</v>
       </c>
       <c r="D22">
-        <v>557.6</v>
+        <v>580.1</v>
       </c>
       <c r="E22">
-        <v>3.3338000000000001</v>
+        <v>2.4632999999999998</v>
       </c>
       <c r="F22">
-        <v>958</v>
+        <v>718</v>
       </c>
       <c r="G22">
-        <v>143.5</v>
+        <v>111.88</v>
       </c>
       <c r="H22">
-        <v>1859</v>
+        <v>1429</v>
       </c>
       <c r="I22" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B23">
         <v>3</v>
       </c>
       <c r="C23" t="s">
         <v>10</v>
+      </c>
+      <c r="D23">
+        <v>565.29999999999995</v>
+      </c>
+      <c r="E23">
+        <v>2.4693999999999998</v>
+      </c>
+      <c r="F23">
+        <v>718</v>
+      </c>
+      <c r="G23">
+        <v>109</v>
+      </c>
+      <c r="H23">
+        <v>1396</v>
+      </c>
+      <c r="I23" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24">
+        <v>559.6</v>
+      </c>
+      <c r="E24">
+        <v>2.4767000000000001</v>
+      </c>
+      <c r="F24">
+        <v>718</v>
+      </c>
+      <c r="G24">
+        <v>108.1</v>
+      </c>
+      <c r="H24">
+        <v>1386</v>
+      </c>
+      <c r="I24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25">
+        <v>546.29999999999995</v>
+      </c>
+      <c r="E25">
+        <v>2.4878999999999998</v>
+      </c>
+      <c r="F25">
+        <v>718</v>
+      </c>
+      <c r="G25">
+        <v>105.3</v>
+      </c>
+      <c r="H25">
+        <v>1359</v>
+      </c>
+      <c r="I25" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26">
+        <v>544.75</v>
+      </c>
+      <c r="E26">
+        <v>2.4897</v>
+      </c>
+      <c r="F26">
+        <v>718</v>
+      </c>
+      <c r="G26">
+        <v>104.9</v>
+      </c>
+      <c r="H26">
+        <v>1353</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27">
+        <v>572.79999999999995</v>
+      </c>
+      <c r="E27">
+        <v>2.4754999999999998</v>
+      </c>
+      <c r="F27">
+        <v>718</v>
+      </c>
+      <c r="G27">
+        <v>109.9</v>
+      </c>
+      <c r="H27">
+        <v>1418</v>
+      </c>
+      <c r="I27" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28">
+        <v>531.77</v>
+      </c>
+      <c r="E28">
+        <v>2.4878999999999998</v>
+      </c>
+      <c r="F28">
+        <v>718</v>
+      </c>
+      <c r="G28">
+        <v>103.35</v>
+      </c>
+      <c r="H28">
+        <v>1323</v>
+      </c>
+      <c r="I28" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29">
+        <v>316.7</v>
+      </c>
+      <c r="E29">
+        <v>1.7334000000000001</v>
+      </c>
+      <c r="F29">
+        <v>478</v>
+      </c>
+      <c r="G29">
+        <v>44.1</v>
+      </c>
+      <c r="H29">
+        <v>549</v>
+      </c>
+      <c r="I29" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30">
+        <v>329.59</v>
+      </c>
+      <c r="E30">
+        <v>1.7263999999999999</v>
+      </c>
+      <c r="F30">
+        <v>478</v>
+      </c>
+      <c r="G30">
+        <v>45.8</v>
+      </c>
+      <c r="H30">
+        <v>569</v>
+      </c>
+      <c r="I30" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31">
+        <v>305.8</v>
+      </c>
+      <c r="E31">
+        <v>1.7362</v>
+      </c>
+      <c r="F31">
+        <v>478</v>
+      </c>
+      <c r="G31">
+        <v>45.5</v>
+      </c>
+      <c r="H31">
+        <v>531</v>
+      </c>
+      <c r="I31" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>66</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32">
+        <v>295.5</v>
+      </c>
+      <c r="E32">
+        <v>1.7427999999999999</v>
+      </c>
+      <c r="F32">
+        <v>478</v>
+      </c>
+      <c r="G32">
+        <v>43.96</v>
+      </c>
+      <c r="H32">
+        <v>515</v>
+      </c>
+      <c r="I32" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33" s="2">
+        <v>5</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" s="2">
+        <v>347</v>
+      </c>
+      <c r="E33" s="2">
+        <v>4.4180999999999999</v>
+      </c>
+      <c r="F33" s="2">
+        <v>1198</v>
+      </c>
+      <c r="G33" s="2">
+        <v>119.72</v>
+      </c>
+      <c r="H33" s="2">
+        <v>1534</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="2">
+        <v>364</v>
+      </c>
+      <c r="E34" s="2">
+        <v>4.3948</v>
+      </c>
+      <c r="F34" s="2">
+        <v>1198</v>
+      </c>
+      <c r="G34" s="2">
+        <v>127.8</v>
+      </c>
+      <c r="H34" s="2">
+        <v>1600</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="2">
+        <v>410</v>
+      </c>
+      <c r="E35" s="2">
+        <v>3.9182000000000001</v>
+      </c>
+      <c r="F35" s="2">
+        <v>1087</v>
+      </c>
+      <c r="G35" s="2">
+        <v>131.24</v>
+      </c>
+      <c r="H35" s="2">
+        <v>1607</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>72</v>
+      </c>
+      <c r="B36">
+        <v>5</v>
+      </c>
+      <c r="C36" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36">
+        <v>1328</v>
+      </c>
+      <c r="E36">
+        <v>3.4908999999999999</v>
+      </c>
+      <c r="F36">
+        <v>1198</v>
+      </c>
+      <c r="G36">
+        <v>360.18</v>
+      </c>
+      <c r="H36">
+        <v>4638</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="J36" t="s">
+        <v>76</v>
+      </c>
+      <c r="K36" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37">
+        <v>5</v>
+      </c>
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" s="3">
+        <v>1334</v>
+      </c>
+      <c r="E37" s="3">
+        <v>3.44</v>
+      </c>
+      <c r="F37" s="3">
+        <v>1198</v>
+      </c>
+      <c r="G37" s="3">
+        <v>356.44</v>
+      </c>
+      <c r="H37" s="3">
+        <v>4590</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B38" s="3">
+        <v>5</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" s="3">
+        <v>1322.8</v>
+      </c>
+      <c r="E38" s="3">
+        <v>3.4495</v>
+      </c>
+      <c r="F38" s="3">
+        <v>1198</v>
+      </c>
+      <c r="G38" s="3">
+        <v>354.6</v>
+      </c>
+      <c r="H38" s="3">
+        <v>4536</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B39" s="3">
+        <v>5</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" s="3">
+        <v>1219.9000000000001</v>
+      </c>
+      <c r="E39" s="3">
+        <v>3.5289999999999999</v>
+      </c>
+      <c r="F39" s="3">
+        <v>1198</v>
+      </c>
+      <c r="G39" s="3">
+        <v>335.22</v>
+      </c>
+      <c r="H39" s="3">
+        <v>4305</v>
+      </c>
+      <c r="I39" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B40" s="3">
+        <v>5</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" s="3">
+        <v>1216.7</v>
+      </c>
+      <c r="E40" s="3">
+        <v>3.5291000000000001</v>
+      </c>
+      <c r="F40" s="3">
+        <v>1198</v>
+      </c>
+      <c r="G40" s="3">
+        <v>336.3</v>
+      </c>
+      <c r="H40" s="3">
+        <v>4294</v>
+      </c>
+      <c r="I40" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B41" s="3">
+        <v>5</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" s="3">
+        <v>1186</v>
+      </c>
+      <c r="E41" s="3">
+        <v>3.5756000000000001</v>
+      </c>
+      <c r="F41" s="3">
+        <v>1198</v>
+      </c>
+      <c r="G41" s="3">
+        <v>329.8</v>
+      </c>
+      <c r="H41" s="3">
+        <v>4243</v>
+      </c>
+      <c r="I41" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished day 2 of exp vert vs horz. frustrated with inconsistent pre and post vert runs.
</commit_message>
<xml_diff>
--- a/Development/IFCB_vehicles/VehicleLabExperimentFiles.xlsx
+++ b/Development/IFCB_vehicles/VehicleLabExperimentFiles.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="101">
   <si>
     <t>Filename</t>
   </si>
@@ -295,6 +295,39 @@
   </si>
   <si>
     <t>pos good, no junk, conc slightly lower</t>
+  </si>
+  <si>
+    <t>D20151104T193427</t>
+  </si>
+  <si>
+    <t>first vert sample after horz</t>
+  </si>
+  <si>
+    <t>D20151104T200201</t>
+  </si>
+  <si>
+    <t>weird shift down in ypos</t>
+  </si>
+  <si>
+    <t>D20151104T202421</t>
+  </si>
+  <si>
+    <t>pos still weird and low</t>
+  </si>
+  <si>
+    <t>D20151104T204641</t>
+  </si>
+  <si>
+    <t>pos stilll lower than usual</t>
+  </si>
+  <si>
+    <t>pos still low, no junk in sample</t>
+  </si>
+  <si>
+    <t>D20151104T210900</t>
+  </si>
+  <si>
+    <t>D20151104T213356</t>
   </si>
 </sst>
 </file>
@@ -917,11 +950,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J42" sqref="J42"/>
+      <selection pane="bottomLeft" activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2164,7 +2197,179 @@
         <v>89</v>
       </c>
     </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B42" s="3">
+        <v>5</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" s="3">
+        <v>1137.8</v>
+      </c>
+      <c r="E42" s="3">
+        <v>3.5983000000000001</v>
+      </c>
+      <c r="F42" s="3">
+        <v>1198</v>
+      </c>
+      <c r="G42" s="3">
+        <v>318.89999999999998</v>
+      </c>
+      <c r="H42" s="3">
+        <v>4094</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B43" s="3">
+        <v>5</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" s="3">
+        <v>1267.9000000000001</v>
+      </c>
+      <c r="E43" s="3">
+        <v>3.4971000000000001</v>
+      </c>
+      <c r="F43" s="3">
+        <v>1198</v>
+      </c>
+      <c r="G43" s="3">
+        <v>343.34</v>
+      </c>
+      <c r="H43" s="3">
+        <v>4434</v>
+      </c>
+      <c r="I43" t="s">
+        <v>91</v>
+      </c>
+      <c r="J43" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B44" s="3">
+        <v>5</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" s="3">
+        <v>1251</v>
+      </c>
+      <c r="E44" s="3">
+        <v>3.5053000000000001</v>
+      </c>
+      <c r="F44" s="3">
+        <v>1198</v>
+      </c>
+      <c r="G44" s="3">
+        <v>340.3</v>
+      </c>
+      <c r="H44" s="3">
+        <v>4385</v>
+      </c>
+      <c r="I44" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B45" s="3">
+        <v>5</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" s="3">
+        <v>1185.7</v>
+      </c>
+      <c r="E45" s="3">
+        <v>3.6105999999999998</v>
+      </c>
+      <c r="F45" s="3">
+        <v>1198</v>
+      </c>
+      <c r="G45" s="3">
+        <v>331.4</v>
+      </c>
+      <c r="H45" s="3">
+        <v>4281</v>
+      </c>
+      <c r="I45" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B46" s="3">
+        <v>5</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" s="3">
+        <v>1222.9000000000001</v>
+      </c>
+      <c r="E46" s="3">
+        <v>3.5324</v>
+      </c>
+      <c r="F46" s="3">
+        <v>1198</v>
+      </c>
+      <c r="G46" s="3">
+        <v>335.3</v>
+      </c>
+      <c r="H46" s="3">
+        <v>4320</v>
+      </c>
+      <c r="I46" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B47" s="3">
+        <v>5</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" s="3">
+        <v>1165.3</v>
+      </c>
+      <c r="E47" s="3">
+        <v>3.6246999999999998</v>
+      </c>
+      <c r="F47" s="3">
+        <v>1198</v>
+      </c>
+      <c r="G47" s="3">
+        <v>328</v>
+      </c>
+      <c r="H47" s="3">
+        <v>4224</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update exp round 3
</commit_message>
<xml_diff>
--- a/Development/IFCB_vehicles/VehicleLabExperimentFiles.xlsx
+++ b/Development/IFCB_vehicles/VehicleLabExperimentFiles.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="108">
   <si>
     <t>Filename</t>
   </si>
@@ -328,6 +328,27 @@
   </si>
   <si>
     <t>D20151104T213356</t>
+  </si>
+  <si>
+    <t>try solution this morning and some clumpy beads so make new solution and add azide this time</t>
+  </si>
+  <si>
+    <t>ypos was low this morning so soak micro 25min</t>
+  </si>
+  <si>
+    <t>D20151105T194435</t>
+  </si>
+  <si>
+    <t>D20151105T200655</t>
+  </si>
+  <si>
+    <t>D20151105T202915</t>
+  </si>
+  <si>
+    <t>ypos consistent through files, no real junk, separate beads</t>
+  </si>
+  <si>
+    <t>D20151105T210041</t>
   </si>
 </sst>
 </file>
@@ -950,11 +971,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K47"/>
+  <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2368,6 +2389,108 @@
         <v>4224</v>
       </c>
     </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I48" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I49" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>103</v>
+      </c>
+      <c r="B50">
+        <v>5</v>
+      </c>
+      <c r="C50" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50">
+        <v>594.57000000000005</v>
+      </c>
+      <c r="E50">
+        <v>4.1223000000000001</v>
+      </c>
+      <c r="F50">
+        <v>1198</v>
+      </c>
+      <c r="G50">
+        <v>191.46</v>
+      </c>
+      <c r="H50">
+        <v>2451</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>104</v>
+      </c>
+      <c r="B51">
+        <v>5</v>
+      </c>
+      <c r="C51" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51">
+        <v>598.27</v>
+      </c>
+      <c r="E51">
+        <v>1.1787000000000001</v>
+      </c>
+      <c r="F51">
+        <v>1198</v>
+      </c>
+      <c r="G51">
+        <v>195.1</v>
+      </c>
+      <c r="H51">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>105</v>
+      </c>
+      <c r="B52">
+        <v>5</v>
+      </c>
+      <c r="C52" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52">
+        <v>585.6</v>
+      </c>
+      <c r="E52">
+        <v>4.1288999999999998</v>
+      </c>
+      <c r="F52">
+        <v>1198</v>
+      </c>
+      <c r="G52">
+        <v>188</v>
+      </c>
+      <c r="H52">
+        <v>2418</v>
+      </c>
+      <c r="I52" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>107</v>
+      </c>
+      <c r="B53">
+        <v>5</v>
+      </c>
+      <c r="C53" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update with exp3 horz runs
</commit_message>
<xml_diff>
--- a/Development/IFCB_vehicles/VehicleLabExperimentFiles.xlsx
+++ b/Development/IFCB_vehicles/VehicleLabExperimentFiles.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\ifcb-analysis\Development\IFCB_vehicles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\from_Samwise\ifcb-analysis\Development\IFCB_vehicles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="113">
   <si>
     <t>Filename</t>
   </si>
@@ -349,6 +349,21 @@
   </si>
   <si>
     <t>D20151105T210041</t>
+  </si>
+  <si>
+    <t>pos consistent as vert, focus tiny off, pmtB signals worse for more ypos when horz?, still not much junk or clustering</t>
+  </si>
+  <si>
+    <t>D20151105T212301</t>
+  </si>
+  <si>
+    <t>same as last</t>
+  </si>
+  <si>
+    <t>D20151105T214520</t>
+  </si>
+  <si>
+    <t>all files look good, slightly lower conc, some a tiny bit out of focus</t>
   </si>
 </sst>
 </file>
@@ -971,11 +986,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K53"/>
+  <dimension ref="A1:K55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D53" sqref="D53"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2394,12 +2409,12 @@
         <v>101</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I49" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>103</v>
       </c>
@@ -2425,7 +2440,7 @@
         <v>2451</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>104</v>
       </c>
@@ -2439,7 +2454,7 @@
         <v>598.27</v>
       </c>
       <c r="E51">
-        <v>1.1787000000000001</v>
+        <v>4.1787000000000001</v>
       </c>
       <c r="F51">
         <v>1198</v>
@@ -2451,7 +2466,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>105</v>
       </c>
@@ -2480,7 +2495,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>107</v>
       </c>
@@ -2489,6 +2504,85 @@
       </c>
       <c r="C53" t="s">
         <v>10</v>
+      </c>
+      <c r="D53">
+        <v>534.47</v>
+      </c>
+      <c r="E53">
+        <v>4.1947999999999999</v>
+      </c>
+      <c r="F53">
+        <v>1198</v>
+      </c>
+      <c r="G53">
+        <v>175.7</v>
+      </c>
+      <c r="H53">
+        <v>2242</v>
+      </c>
+      <c r="I53" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>109</v>
+      </c>
+      <c r="B54">
+        <v>5</v>
+      </c>
+      <c r="C54" t="s">
+        <v>10</v>
+      </c>
+      <c r="D54">
+        <v>560.29999999999995</v>
+      </c>
+      <c r="E54">
+        <v>4.2214</v>
+      </c>
+      <c r="F54">
+        <v>1198</v>
+      </c>
+      <c r="G54">
+        <v>184.58</v>
+      </c>
+      <c r="H54">
+        <v>2366</v>
+      </c>
+      <c r="I54" t="s">
+        <v>110</v>
+      </c>
+      <c r="J54" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>111</v>
+      </c>
+      <c r="B55">
+        <v>5</v>
+      </c>
+      <c r="C55" t="s">
+        <v>10</v>
+      </c>
+      <c r="D55">
+        <v>524.5</v>
+      </c>
+      <c r="E55">
+        <v>4.2076000000000002</v>
+      </c>
+      <c r="F55">
+        <v>1198</v>
+      </c>
+      <c r="G55">
+        <v>171.6</v>
+      </c>
+      <c r="H55">
+        <v>2207</v>
+      </c>
+      <c r="I55" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished round 3 of cellconc in vert vs horz
</commit_message>
<xml_diff>
--- a/Development/IFCB_vehicles/VehicleLabExperimentFiles.xlsx
+++ b/Development/IFCB_vehicles/VehicleLabExperimentFiles.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="130">
   <si>
     <t>Filename</t>
   </si>
@@ -364,6 +364,57 @@
   </si>
   <si>
     <t>all files look good, slightly lower conc, some a tiny bit out of focus</t>
+  </si>
+  <si>
+    <t>D20151105T221748</t>
+  </si>
+  <si>
+    <t>lots of missed rois, ypos when way high halfway out of FOV</t>
+  </si>
+  <si>
+    <t>no clumps of junk, cellconc use all signals, does it calculate conc including zerosize rois?</t>
+  </si>
+  <si>
+    <t>D20151105T224008</t>
+  </si>
+  <si>
+    <t>still lots of missed rois, high ypos off FOV ~450-1030</t>
+  </si>
+  <si>
+    <t>no junk or visible bubbles</t>
+  </si>
+  <si>
+    <t>from pmtAvsB most of missed rois show signals that they're beads and just out of camera sight</t>
+  </si>
+  <si>
+    <t>ypos still high off top but not as many missed, 300-1030</t>
+  </si>
+  <si>
+    <t>no junk, slightly more bead doublets</t>
+  </si>
+  <si>
+    <t>D20151105T230227</t>
+  </si>
+  <si>
+    <t>length(tind)=26 which is really weird because a lot of very high ypos</t>
+  </si>
+  <si>
+    <t>length(tind)=310</t>
+  </si>
+  <si>
+    <t>length(tind)=782</t>
+  </si>
+  <si>
+    <t>D20151105T232446</t>
+  </si>
+  <si>
+    <t>ypos high but core completely in FOV, a few tiny pieces of junk and doublets and triplets but no large clumps, seems acceptable</t>
+  </si>
+  <si>
+    <t>length(tind)=12</t>
+  </si>
+  <si>
+    <t>fresh bead in FSW just made to start over</t>
   </si>
 </sst>
 </file>
@@ -986,11 +1037,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K55"/>
+  <dimension ref="A1:L60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D56" sqref="D56"/>
+      <selection pane="bottomLeft" activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2053,94 +2104,70 @@
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>72</v>
-      </c>
-      <c r="B36">
-        <v>5</v>
-      </c>
-      <c r="C36" t="s">
-        <v>5</v>
-      </c>
-      <c r="D36">
-        <v>1328</v>
-      </c>
-      <c r="E36">
-        <v>3.4908999999999999</v>
-      </c>
-      <c r="F36">
-        <v>1198</v>
-      </c>
-      <c r="G36">
-        <v>360.18</v>
-      </c>
-      <c r="H36">
-        <v>4638</v>
-      </c>
+    <row r="36" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="I36" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="J36" t="s">
-        <v>76</v>
-      </c>
-      <c r="K36" t="s">
-        <v>37</v>
+        <v>129</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37">
+        <v>5</v>
+      </c>
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37">
+        <v>1328</v>
+      </c>
+      <c r="E37">
+        <v>3.4908999999999999</v>
+      </c>
+      <c r="F37">
+        <v>1198</v>
+      </c>
+      <c r="G37">
+        <v>360.18</v>
+      </c>
+      <c r="H37">
+        <v>4638</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="J37" t="s">
+        <v>76</v>
+      </c>
+      <c r="K37" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>73</v>
       </c>
-      <c r="B37">
-        <v>5</v>
-      </c>
-      <c r="C37" t="s">
-        <v>5</v>
-      </c>
-      <c r="D37" s="3">
+      <c r="B38">
+        <v>5</v>
+      </c>
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" s="3">
         <v>1334</v>
       </c>
-      <c r="E37" s="3">
+      <c r="E38" s="3">
         <v>3.44</v>
       </c>
-      <c r="F37" s="3">
-        <v>1198</v>
-      </c>
-      <c r="G37" s="3">
+      <c r="F38" s="3">
+        <v>1198</v>
+      </c>
+      <c r="G38" s="3">
         <v>356.44</v>
       </c>
-      <c r="H37" s="3">
+      <c r="H38" s="3">
         <v>4590</v>
-      </c>
-      <c r="I37" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B38" s="3">
-        <v>5</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" s="3">
-        <v>1322.8</v>
-      </c>
-      <c r="E38" s="3">
-        <v>3.4495</v>
-      </c>
-      <c r="F38" s="3">
-        <v>1198</v>
-      </c>
-      <c r="G38" s="3">
-        <v>354.6</v>
-      </c>
-      <c r="H38" s="3">
-        <v>4536</v>
       </c>
       <c r="I38" s="3" t="s">
         <v>37</v>
@@ -2148,36 +2175,36 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B39" s="3">
         <v>5</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D39" s="3">
-        <v>1219.9000000000001</v>
+        <v>1322.8</v>
       </c>
       <c r="E39" s="3">
-        <v>3.5289999999999999</v>
+        <v>3.4495</v>
       </c>
       <c r="F39" s="3">
         <v>1198</v>
       </c>
       <c r="G39" s="3">
-        <v>335.22</v>
+        <v>354.6</v>
       </c>
       <c r="H39" s="3">
-        <v>4305</v>
-      </c>
-      <c r="I39" t="s">
-        <v>78</v>
+        <v>4536</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B40" s="3">
         <v>5</v>
@@ -2186,27 +2213,27 @@
         <v>10</v>
       </c>
       <c r="D40" s="3">
-        <v>1216.7</v>
+        <v>1219.9000000000001</v>
       </c>
       <c r="E40" s="3">
-        <v>3.5291000000000001</v>
+        <v>3.5289999999999999</v>
       </c>
       <c r="F40" s="3">
         <v>1198</v>
       </c>
       <c r="G40" s="3">
-        <v>336.3</v>
+        <v>335.22</v>
       </c>
       <c r="H40" s="3">
-        <v>4294</v>
+        <v>4305</v>
       </c>
       <c r="I40" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B41" s="3">
         <v>5</v>
@@ -2215,27 +2242,27 @@
         <v>10</v>
       </c>
       <c r="D41" s="3">
-        <v>1186</v>
+        <v>1216.7</v>
       </c>
       <c r="E41" s="3">
-        <v>3.5756000000000001</v>
+        <v>3.5291000000000001</v>
       </c>
       <c r="F41" s="3">
         <v>1198</v>
       </c>
       <c r="G41" s="3">
-        <v>329.8</v>
+        <v>336.3</v>
       </c>
       <c r="H41" s="3">
-        <v>4243</v>
+        <v>4294</v>
       </c>
       <c r="I41" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B42" s="3">
         <v>5</v>
@@ -2244,56 +2271,53 @@
         <v>10</v>
       </c>
       <c r="D42" s="3">
-        <v>1137.8</v>
+        <v>1186</v>
       </c>
       <c r="E42" s="3">
-        <v>3.5983000000000001</v>
+        <v>3.5756000000000001</v>
       </c>
       <c r="F42" s="3">
         <v>1198</v>
       </c>
       <c r="G42" s="3">
-        <v>318.89999999999998</v>
+        <v>329.8</v>
       </c>
       <c r="H42" s="3">
-        <v>4094</v>
+        <v>4243</v>
+      </c>
+      <c r="I42" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B43" s="3">
         <v>5</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D43" s="3">
-        <v>1267.9000000000001</v>
+        <v>1137.8</v>
       </c>
       <c r="E43" s="3">
-        <v>3.4971000000000001</v>
+        <v>3.5983000000000001</v>
       </c>
       <c r="F43" s="3">
         <v>1198</v>
       </c>
       <c r="G43" s="3">
-        <v>343.34</v>
+        <v>318.89999999999998</v>
       </c>
       <c r="H43" s="3">
-        <v>4434</v>
-      </c>
-      <c r="I43" t="s">
-        <v>91</v>
-      </c>
-      <c r="J43" t="s">
-        <v>93</v>
+        <v>4094</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B44" s="3">
         <v>5</v>
@@ -2302,27 +2326,30 @@
         <v>5</v>
       </c>
       <c r="D44" s="3">
-        <v>1251</v>
+        <v>1267.9000000000001</v>
       </c>
       <c r="E44" s="3">
-        <v>3.5053000000000001</v>
+        <v>3.4971000000000001</v>
       </c>
       <c r="F44" s="3">
         <v>1198</v>
       </c>
       <c r="G44" s="3">
-        <v>340.3</v>
+        <v>343.34</v>
       </c>
       <c r="H44" s="3">
-        <v>4385</v>
+        <v>4434</v>
       </c>
       <c r="I44" t="s">
-        <v>95</v>
+        <v>91</v>
+      </c>
+      <c r="J44" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B45" s="3">
         <v>5</v>
@@ -2331,27 +2358,27 @@
         <v>5</v>
       </c>
       <c r="D45" s="3">
-        <v>1185.7</v>
+        <v>1251</v>
       </c>
       <c r="E45" s="3">
-        <v>3.6105999999999998</v>
+        <v>3.5053000000000001</v>
       </c>
       <c r="F45" s="3">
         <v>1198</v>
       </c>
       <c r="G45" s="3">
-        <v>331.4</v>
+        <v>340.3</v>
       </c>
       <c r="H45" s="3">
-        <v>4281</v>
+        <v>4385</v>
       </c>
       <c r="I45" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B46" s="3">
         <v>5</v>
@@ -2360,229 +2387,398 @@
         <v>5</v>
       </c>
       <c r="D46" s="3">
-        <v>1222.9000000000001</v>
+        <v>1185.7</v>
       </c>
       <c r="E46" s="3">
-        <v>3.5324</v>
+        <v>3.6105999999999998</v>
       </c>
       <c r="F46" s="3">
         <v>1198</v>
       </c>
       <c r="G46" s="3">
-        <v>335.3</v>
+        <v>331.4</v>
       </c>
       <c r="H46" s="3">
-        <v>4320</v>
+        <v>4281</v>
       </c>
       <c r="I46" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B47" s="3">
+        <v>5</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" s="3">
+        <v>1222.9000000000001</v>
+      </c>
+      <c r="E47" s="3">
+        <v>3.5324</v>
+      </c>
+      <c r="F47" s="3">
+        <v>1198</v>
+      </c>
+      <c r="G47" s="3">
+        <v>335.3</v>
+      </c>
+      <c r="H47" s="3">
+        <v>4320</v>
+      </c>
+      <c r="I47" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B47" s="3">
-        <v>5</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D47" s="3">
+      <c r="B48" s="3">
+        <v>5</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" s="3">
         <v>1165.3</v>
       </c>
-      <c r="E47" s="3">
+      <c r="E48" s="3">
         <v>3.6246999999999998</v>
       </c>
-      <c r="F47" s="3">
-        <v>1198</v>
-      </c>
-      <c r="G47" s="3">
+      <c r="F48" s="3">
+        <v>1198</v>
+      </c>
+      <c r="G48" s="3">
         <v>328</v>
       </c>
-      <c r="H47" s="3">
+      <c r="H48" s="3">
         <v>4224</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I48" t="s">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I49" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I49" t="s">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I50" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>103</v>
       </c>
-      <c r="B50">
-        <v>5</v>
-      </c>
-      <c r="C50" t="s">
-        <v>5</v>
-      </c>
-      <c r="D50">
+      <c r="B51">
+        <v>5</v>
+      </c>
+      <c r="C51" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51">
         <v>594.57000000000005</v>
       </c>
-      <c r="E50">
+      <c r="E51">
         <v>4.1223000000000001</v>
       </c>
-      <c r="F50">
-        <v>1198</v>
-      </c>
-      <c r="G50">
+      <c r="F51">
+        <v>1198</v>
+      </c>
+      <c r="G51">
         <v>191.46</v>
       </c>
-      <c r="H50">
+      <c r="H51">
         <v>2451</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>104</v>
       </c>
-      <c r="B51">
-        <v>5</v>
-      </c>
-      <c r="C51" t="s">
-        <v>5</v>
-      </c>
-      <c r="D51">
+      <c r="B52">
+        <v>5</v>
+      </c>
+      <c r="C52" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52">
         <v>598.27</v>
       </c>
-      <c r="E51">
+      <c r="E52">
         <v>4.1787000000000001</v>
       </c>
-      <c r="F51">
-        <v>1198</v>
-      </c>
-      <c r="G51">
+      <c r="F52">
+        <v>1198</v>
+      </c>
+      <c r="G52">
         <v>195.1</v>
       </c>
-      <c r="H51">
+      <c r="H52">
         <v>2500</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>105</v>
       </c>
-      <c r="B52">
-        <v>5</v>
-      </c>
-      <c r="C52" t="s">
-        <v>5</v>
-      </c>
-      <c r="D52">
+      <c r="B53">
+        <v>5</v>
+      </c>
+      <c r="C53" t="s">
+        <v>5</v>
+      </c>
+      <c r="D53">
         <v>585.6</v>
       </c>
-      <c r="E52">
+      <c r="E53">
         <v>4.1288999999999998</v>
       </c>
-      <c r="F52">
-        <v>1198</v>
-      </c>
-      <c r="G52">
+      <c r="F53">
+        <v>1198</v>
+      </c>
+      <c r="G53">
         <v>188</v>
       </c>
-      <c r="H52">
+      <c r="H53">
         <v>2418</v>
       </c>
-      <c r="I52" t="s">
+      <c r="I53" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>107</v>
       </c>
-      <c r="B53">
-        <v>5</v>
-      </c>
-      <c r="C53" t="s">
-        <v>10</v>
-      </c>
-      <c r="D53">
+      <c r="B54">
+        <v>5</v>
+      </c>
+      <c r="C54" t="s">
+        <v>10</v>
+      </c>
+      <c r="D54">
         <v>534.47</v>
       </c>
-      <c r="E53">
+      <c r="E54">
         <v>4.1947999999999999</v>
       </c>
-      <c r="F53">
-        <v>1198</v>
-      </c>
-      <c r="G53">
+      <c r="F54">
+        <v>1198</v>
+      </c>
+      <c r="G54">
         <v>175.7</v>
       </c>
-      <c r="H53">
+      <c r="H54">
         <v>2242</v>
       </c>
-      <c r="I53" t="s">
+      <c r="I54" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>109</v>
       </c>
-      <c r="B54">
-        <v>5</v>
-      </c>
-      <c r="C54" t="s">
-        <v>10</v>
-      </c>
-      <c r="D54">
+      <c r="B55">
+        <v>5</v>
+      </c>
+      <c r="C55" t="s">
+        <v>10</v>
+      </c>
+      <c r="D55">
         <v>560.29999999999995</v>
       </c>
-      <c r="E54">
+      <c r="E55">
         <v>4.2214</v>
       </c>
-      <c r="F54">
-        <v>1198</v>
-      </c>
-      <c r="G54">
+      <c r="F55">
+        <v>1198</v>
+      </c>
+      <c r="G55">
         <v>184.58</v>
       </c>
-      <c r="H54">
+      <c r="H55">
         <v>2366</v>
       </c>
-      <c r="I54" t="s">
+      <c r="I55" t="s">
         <v>110</v>
       </c>
-      <c r="J54" t="s">
+      <c r="J55" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>111</v>
       </c>
-      <c r="B55">
-        <v>5</v>
-      </c>
-      <c r="C55" t="s">
-        <v>10</v>
-      </c>
-      <c r="D55">
+      <c r="B56">
+        <v>5</v>
+      </c>
+      <c r="C56" t="s">
+        <v>10</v>
+      </c>
+      <c r="D56">
         <v>524.5</v>
       </c>
-      <c r="E55">
+      <c r="E56">
         <v>4.2076000000000002</v>
       </c>
-      <c r="F55">
-        <v>1198</v>
-      </c>
-      <c r="G55">
+      <c r="F56">
+        <v>1198</v>
+      </c>
+      <c r="G56">
         <v>171.6</v>
       </c>
-      <c r="H55">
+      <c r="H56">
         <v>2207</v>
       </c>
-      <c r="I55" t="s">
+      <c r="I56" t="s">
         <v>112</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>113</v>
+      </c>
+      <c r="B57">
+        <v>5</v>
+      </c>
+      <c r="C57" t="s">
+        <v>5</v>
+      </c>
+      <c r="D57">
+        <v>610.6</v>
+      </c>
+      <c r="E57">
+        <v>4.1073000000000004</v>
+      </c>
+      <c r="F57">
+        <v>1198</v>
+      </c>
+      <c r="G57">
+        <v>196.7</v>
+      </c>
+      <c r="H57">
+        <v>2508</v>
+      </c>
+      <c r="I57" t="s">
+        <v>114</v>
+      </c>
+      <c r="J57" t="s">
+        <v>115</v>
+      </c>
+      <c r="K57" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>116</v>
+      </c>
+      <c r="B58">
+        <v>5</v>
+      </c>
+      <c r="C58" t="s">
+        <v>5</v>
+      </c>
+      <c r="D58">
+        <v>596.29999999999995</v>
+      </c>
+      <c r="E58">
+        <v>4.1288999999999998</v>
+      </c>
+      <c r="F58">
+        <v>1198</v>
+      </c>
+      <c r="G58">
+        <v>191.1</v>
+      </c>
+      <c r="H58">
+        <v>2462</v>
+      </c>
+      <c r="I58" t="s">
+        <v>117</v>
+      </c>
+      <c r="J58" t="s">
+        <v>118</v>
+      </c>
+      <c r="K58" t="s">
+        <v>119</v>
+      </c>
+      <c r="L58" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>122</v>
+      </c>
+      <c r="B59">
+        <v>5</v>
+      </c>
+      <c r="C59" t="s">
+        <v>5</v>
+      </c>
+      <c r="D59">
+        <v>598.79999999999995</v>
+      </c>
+      <c r="E59">
+        <v>4.1215000000000002</v>
+      </c>
+      <c r="F59">
+        <v>1198</v>
+      </c>
+      <c r="G59">
+        <v>192.3</v>
+      </c>
+      <c r="H59">
+        <v>2468</v>
+      </c>
+      <c r="I59" t="s">
+        <v>120</v>
+      </c>
+      <c r="J59" t="s">
+        <v>121</v>
+      </c>
+      <c r="K59" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>126</v>
+      </c>
+      <c r="B60">
+        <v>5</v>
+      </c>
+      <c r="C60" t="s">
+        <v>5</v>
+      </c>
+      <c r="D60">
+        <v>576.70000000000005</v>
+      </c>
+      <c r="E60">
+        <v>4.1475</v>
+      </c>
+      <c r="F60">
+        <v>1198</v>
+      </c>
+      <c r="G60">
+        <v>186.5</v>
+      </c>
+      <c r="H60">
+        <v>2392</v>
+      </c>
+      <c r="I60" t="s">
+        <v>127</v>
+      </c>
+      <c r="J60" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more exp updated 1ml and 3ml h vs v
</commit_message>
<xml_diff>
--- a/Development/IFCB_vehicles/VehicleLabExperimentFiles.xlsx
+++ b/Development/IFCB_vehicles/VehicleLabExperimentFiles.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\from_Samwise\ifcb-analysis\Development\IFCB_vehicles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\ifcb-analysis\Development\IFCB_vehicles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="235">
   <si>
     <t>Filename</t>
   </si>
@@ -415,13 +415,328 @@
   </si>
   <si>
     <t>fresh bead in FSW just made to start over</t>
+  </si>
+  <si>
+    <t>okay, what happens when we run less volume of vert vs horz? Is it less of a differece if our hypothesis is correct?  Should probably make more concentrated beads</t>
+  </si>
+  <si>
+    <t>D20151106T165810</t>
+  </si>
+  <si>
+    <t>D20151106T170409</t>
+  </si>
+  <si>
+    <t>good ypos, clean single beads</t>
+  </si>
+  <si>
+    <t>good typical ypos 150-850, clean single beads</t>
+  </si>
+  <si>
+    <t>D20151106T171009</t>
+  </si>
+  <si>
+    <t>first debubble had a few small bubbles come ou</t>
+  </si>
+  <si>
+    <t>D20151106T171609</t>
+  </si>
+  <si>
+    <t>D20151106T172529</t>
+  </si>
+  <si>
+    <t>D20151106T173129</t>
+  </si>
+  <si>
+    <t>pos still good</t>
+  </si>
+  <si>
+    <t>D20151106T173728</t>
+  </si>
+  <si>
+    <t>pos good, single beads, why'd conc go down so much???</t>
+  </si>
+  <si>
+    <t>D20151106T174328</t>
+  </si>
+  <si>
+    <t>D20151106T175234</t>
+  </si>
+  <si>
+    <t>consistent ypos, no missed rois, clean single beads</t>
+  </si>
+  <si>
+    <t>D20151106T175834</t>
+  </si>
+  <si>
+    <t>D20151106T180434</t>
+  </si>
+  <si>
+    <t>D20151106T181034</t>
+  </si>
+  <si>
+    <t>singles clean</t>
+  </si>
+  <si>
+    <t>D20151106T183213</t>
+  </si>
+  <si>
+    <t>sat about 15-20 min not running</t>
+  </si>
+  <si>
+    <t>D20151106T182613</t>
+  </si>
+  <si>
+    <t>D20151106T184909</t>
+  </si>
+  <si>
+    <t>D20151106T184309</t>
+  </si>
+  <si>
+    <t>D20151106T185928</t>
+  </si>
+  <si>
+    <t>pos still good, clean single beaeds</t>
+  </si>
+  <si>
+    <t>D20151106T190528</t>
+  </si>
+  <si>
+    <t>D20151106T191128</t>
+  </si>
+  <si>
+    <t>D20151106T191728</t>
+  </si>
+  <si>
+    <t>pos good, no junk</t>
+  </si>
+  <si>
+    <t>ypos way down missed 180 off FOV, focus ok, single beads</t>
+  </si>
+  <si>
+    <t>D20151106T192541</t>
+  </si>
+  <si>
+    <t>D20151106T193141</t>
+  </si>
+  <si>
+    <t>ypos even worse almost completely off fov</t>
+  </si>
+  <si>
+    <t>ypos0-150</t>
+  </si>
+  <si>
+    <t>view images 520-535</t>
+  </si>
+  <si>
+    <t>D20151106T193741</t>
+  </si>
+  <si>
+    <t>ypos bad</t>
+  </si>
+  <si>
+    <t>D20151106T200824</t>
+  </si>
+  <si>
+    <t>after beads run, run 5ml twice and 2 debubble to try and flush extra beads away</t>
+  </si>
+  <si>
+    <t>D20151106T204549</t>
+  </si>
+  <si>
+    <t>concentrate beads more</t>
+  </si>
+  <si>
+    <t>good pos, clean bears</t>
+  </si>
+  <si>
+    <t>D20151106T205147</t>
+  </si>
+  <si>
+    <t>D20151106T205747</t>
+  </si>
+  <si>
+    <t>all good</t>
+  </si>
+  <si>
+    <t>D20151106T210347</t>
+  </si>
+  <si>
+    <t>D20151106T212126</t>
+  </si>
+  <si>
+    <t>D20151106T211107</t>
+  </si>
+  <si>
+    <t>D20151106T212725</t>
+  </si>
+  <si>
+    <t>D20151106T213325</t>
+  </si>
+  <si>
+    <t>D20151106T213925</t>
+  </si>
+  <si>
+    <t>D20151106T215008</t>
+  </si>
+  <si>
+    <t>D20151106T215608</t>
+  </si>
+  <si>
+    <t>D20151106T220208</t>
+  </si>
+  <si>
+    <t>D20151106T220808</t>
+  </si>
+  <si>
+    <t>all still good</t>
+  </si>
+  <si>
+    <t>D20151106T221408</t>
+  </si>
+  <si>
+    <t>D20151106T222008</t>
+  </si>
+  <si>
+    <t>Try more concentrated beads at different volumes of V vs H. 1ml seems to matchup, but 5ml not with beads. At what volume? Do more concentrated for better statistics says Rob</t>
+  </si>
+  <si>
+    <t>D20151110T183541</t>
+  </si>
+  <si>
+    <t>pos good</t>
+  </si>
+  <si>
+    <t>D20151110T184951</t>
+  </si>
+  <si>
+    <t>D20151110T190401</t>
+  </si>
+  <si>
+    <t>fair number of doublets but mostly singlets</t>
+  </si>
+  <si>
+    <t>same as previous</t>
+  </si>
+  <si>
+    <t>D20151110T192143</t>
+  </si>
+  <si>
+    <t>pos good, signals same, still a few doublets</t>
+  </si>
+  <si>
+    <t>that's weird, almost same number of triggers but 100cell/ml less because of look time….?</t>
+  </si>
+  <si>
+    <t>D20151110T193553</t>
+  </si>
+  <si>
+    <t>D20151110T195003</t>
+  </si>
+  <si>
+    <t>pos good. Some junk but nothing giant and no clusters of beads besides typical doublet's I've been seeing</t>
+  </si>
+  <si>
+    <t>D20151110T202517</t>
+  </si>
+  <si>
+    <t>D20151110T203926</t>
+  </si>
+  <si>
+    <t>D20151110T205336</t>
+  </si>
+  <si>
+    <t>D20151110T213232</t>
+  </si>
+  <si>
+    <t>Try 1ml volume again with the higher concentration</t>
+  </si>
+  <si>
+    <t>D20151110T213832</t>
+  </si>
+  <si>
+    <t>D20151110T214432</t>
+  </si>
+  <si>
+    <t>D20151110T215032</t>
+  </si>
+  <si>
+    <t>D20151110T215632</t>
+  </si>
+  <si>
+    <t>good pos and pics and singlets</t>
+  </si>
+  <si>
+    <t>good pos singlets</t>
+  </si>
+  <si>
+    <t>good pos, singles with some triplets</t>
+  </si>
+  <si>
+    <t>SAT FOR A WHILE I THINK HIGHER CONC NOT ALL BEADS GETTING SUCKED AWAY BY DEBUBBLE, BECAUSE THIS FIRST RUN IS LOWER BUT 2ND IS NORMAL</t>
+  </si>
+  <si>
+    <t>pos good, focus good, more triplets and now some 4 clusters? But only last run was weird</t>
+  </si>
+  <si>
+    <t>D20151110T220525</t>
+  </si>
+  <si>
+    <t>D20151110T221125</t>
+  </si>
+  <si>
+    <t>D20151110T221725</t>
+  </si>
+  <si>
+    <t>D20151110T222325</t>
+  </si>
+  <si>
+    <t>D20151110T222925</t>
+  </si>
+  <si>
+    <t>pos good, no real junk like bad runs we threw out a couple days ago</t>
+  </si>
+  <si>
+    <t>pos ok rois ok</t>
+  </si>
+  <si>
+    <t>all ok, weird up/down conc;s</t>
+  </si>
+  <si>
+    <t>D20151110T223814</t>
+  </si>
+  <si>
+    <t>D20151110T224414</t>
+  </si>
+  <si>
+    <t>D20151110T225014</t>
+  </si>
+  <si>
+    <t>bubble as first roi</t>
+  </si>
+  <si>
+    <t>other than first roi pos is good and some junk but not a ton and conc actually isn't terrible…</t>
+  </si>
+  <si>
+    <t>beads sort of starting to get clumpy, no air</t>
+  </si>
+  <si>
+    <t>D20151110T225614</t>
+  </si>
+  <si>
+    <t>pos good, a few clumps</t>
+  </si>
+  <si>
+    <t>D201511010T230214</t>
+  </si>
+  <si>
+    <t>all look good</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -429,8 +744,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -440,6 +762,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -456,13 +784,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1037,16 +1367,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L60"/>
+  <dimension ref="A1:L134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I37" sqref="I37"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I135" sqref="I135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
@@ -1057,7 +1387,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -1089,7 +1419,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B2" t="s">
@@ -1124,7 +1454,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B3">
@@ -1156,7 +1486,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B4">
@@ -1188,7 +1518,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B5">
@@ -1220,7 +1550,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B6">
@@ -1252,7 +1582,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B7">
@@ -1284,7 +1614,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B8">
@@ -1319,7 +1649,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B9">
@@ -1348,7 +1678,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B10">
@@ -1377,7 +1707,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B11">
@@ -1406,7 +1736,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B12">
@@ -1435,7 +1765,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B13">
@@ -1464,7 +1794,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B14">
@@ -1496,7 +1826,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B15">
@@ -1525,7 +1855,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B16">
@@ -1554,7 +1884,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B17">
@@ -1583,7 +1913,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B18">
@@ -1612,7 +1942,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B19">
@@ -1641,7 +1971,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="3" t="s">
         <v>54</v>
       </c>
       <c r="B20">
@@ -1670,7 +2000,7 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="3" t="s">
         <v>55</v>
       </c>
       <c r="B21">
@@ -1702,7 +2032,7 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="3" t="s">
         <v>56</v>
       </c>
       <c r="B22">
@@ -1731,7 +2061,7 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="3" t="s">
         <v>57</v>
       </c>
       <c r="B23">
@@ -1760,7 +2090,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B24">
@@ -1789,7 +2119,7 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B25">
@@ -1818,7 +2148,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="3" t="s">
         <v>60</v>
       </c>
       <c r="B26">
@@ -1844,7 +2174,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="3" t="s">
         <v>61</v>
       </c>
       <c r="B27">
@@ -1873,7 +2203,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="3" t="s">
         <v>62</v>
       </c>
       <c r="B28">
@@ -1902,7 +2232,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="3" t="s">
         <v>63</v>
       </c>
       <c r="B29">
@@ -1931,7 +2261,7 @@
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="3" t="s">
         <v>64</v>
       </c>
       <c r="B30">
@@ -1960,7 +2290,7 @@
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="3" t="s">
         <v>65</v>
       </c>
       <c r="B31">
@@ -1989,7 +2319,7 @@
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B32">
@@ -2018,7 +2348,7 @@
       </c>
     </row>
     <row r="33" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="3" t="s">
         <v>67</v>
       </c>
       <c r="B33" s="2">
@@ -2050,7 +2380,7 @@
       </c>
     </row>
     <row r="34" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="3" t="s">
         <v>74</v>
       </c>
       <c r="C34" s="2" t="s">
@@ -2076,7 +2406,7 @@
       </c>
     </row>
     <row r="35" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="3" t="s">
         <v>69</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -2110,7 +2440,7 @@
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="A37" s="3" t="s">
         <v>72</v>
       </c>
       <c r="B37">
@@ -2145,7 +2475,7 @@
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="A38" s="3" t="s">
         <v>73</v>
       </c>
       <c r="B38">
@@ -2471,7 +2801,7 @@
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="A51" s="3" t="s">
         <v>103</v>
       </c>
       <c r="B51">
@@ -2497,7 +2827,7 @@
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="A52" s="3" t="s">
         <v>104</v>
       </c>
       <c r="B52">
@@ -2523,7 +2853,7 @@
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="A53" s="3" t="s">
         <v>105</v>
       </c>
       <c r="B53">
@@ -2552,7 +2882,7 @@
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="A54" s="3" t="s">
         <v>107</v>
       </c>
       <c r="B54">
@@ -2581,7 +2911,7 @@
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="A55" s="3" t="s">
         <v>109</v>
       </c>
       <c r="B55">
@@ -2613,7 +2943,7 @@
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="A56" s="3" t="s">
         <v>111</v>
       </c>
       <c r="B56">
@@ -2642,7 +2972,7 @@
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="A57" s="3" t="s">
         <v>113</v>
       </c>
       <c r="B57">
@@ -2677,7 +3007,7 @@
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="A58" s="3" t="s">
         <v>116</v>
       </c>
       <c r="B58">
@@ -2715,7 +3045,7 @@
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="A59" s="3" t="s">
         <v>122</v>
       </c>
       <c r="B59">
@@ -2750,7 +3080,7 @@
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="A60" s="3" t="s">
         <v>126</v>
       </c>
       <c r="B60">
@@ -2779,6 +3109,1810 @@
       </c>
       <c r="J60" t="s">
         <v>128</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="C63" t="s">
+        <v>5</v>
+      </c>
+      <c r="D63">
+        <v>725</v>
+      </c>
+      <c r="E63">
+        <v>0.80420000000000003</v>
+      </c>
+      <c r="F63">
+        <v>238</v>
+      </c>
+      <c r="G63">
+        <v>45</v>
+      </c>
+      <c r="H63">
+        <v>583</v>
+      </c>
+      <c r="I63" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B64">
+        <v>1</v>
+      </c>
+      <c r="C64" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64">
+        <v>718.46</v>
+      </c>
+      <c r="E64">
+        <v>0.753</v>
+      </c>
+      <c r="F64">
+        <v>238</v>
+      </c>
+      <c r="G64">
+        <v>41.811</v>
+      </c>
+      <c r="H64">
+        <v>541</v>
+      </c>
+      <c r="I64" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B65">
+        <v>1</v>
+      </c>
+      <c r="C65" t="s">
+        <v>5</v>
+      </c>
+      <c r="D65">
+        <v>680</v>
+      </c>
+      <c r="E65">
+        <v>0.76139999999999997</v>
+      </c>
+      <c r="F65">
+        <v>238</v>
+      </c>
+      <c r="G65">
+        <v>40.020000000000003</v>
+      </c>
+      <c r="H65">
+        <v>518</v>
+      </c>
+      <c r="I65" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B66">
+        <v>1</v>
+      </c>
+      <c r="C66" t="s">
+        <v>5</v>
+      </c>
+      <c r="D66">
+        <v>705</v>
+      </c>
+      <c r="E66">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="F66">
+        <v>238</v>
+      </c>
+      <c r="G66">
+        <v>41.99</v>
+      </c>
+      <c r="H66">
+        <v>533</v>
+      </c>
+      <c r="I66" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B67">
+        <v>1</v>
+      </c>
+      <c r="C67" t="s">
+        <v>10</v>
+      </c>
+      <c r="D67">
+        <v>716.7</v>
+      </c>
+      <c r="E67">
+        <v>0.752</v>
+      </c>
+      <c r="F67">
+        <v>238</v>
+      </c>
+      <c r="G67">
+        <v>41.6</v>
+      </c>
+      <c r="H67">
+        <v>539</v>
+      </c>
+      <c r="I67" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B68">
+        <v>1</v>
+      </c>
+      <c r="C68" t="s">
+        <v>10</v>
+      </c>
+      <c r="D68">
+        <v>682</v>
+      </c>
+      <c r="E68">
+        <v>0.75949999999999995</v>
+      </c>
+      <c r="F68">
+        <v>238</v>
+      </c>
+      <c r="G68">
+        <v>40.130000000000003</v>
+      </c>
+      <c r="H68">
+        <v>518</v>
+      </c>
+      <c r="I68" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B69">
+        <v>1</v>
+      </c>
+      <c r="C69" t="s">
+        <v>10</v>
+      </c>
+      <c r="D69">
+        <v>599</v>
+      </c>
+      <c r="E69">
+        <v>0.83130000000000004</v>
+      </c>
+      <c r="F69">
+        <v>238</v>
+      </c>
+      <c r="G69">
+        <v>38.44</v>
+      </c>
+      <c r="H69">
+        <v>498</v>
+      </c>
+      <c r="I69" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B70">
+        <v>1</v>
+      </c>
+      <c r="C70" t="s">
+        <v>10</v>
+      </c>
+      <c r="D70">
+        <v>627.70000000000005</v>
+      </c>
+      <c r="E70">
+        <v>0.82520000000000004</v>
+      </c>
+      <c r="F70">
+        <v>238</v>
+      </c>
+      <c r="G70">
+        <v>39.89</v>
+      </c>
+      <c r="H70">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B71">
+        <v>1</v>
+      </c>
+      <c r="C71" t="s">
+        <v>5</v>
+      </c>
+      <c r="D71">
+        <v>683.65</v>
+      </c>
+      <c r="E71">
+        <v>0.75480000000000003</v>
+      </c>
+      <c r="F71">
+        <v>238</v>
+      </c>
+      <c r="G71">
+        <v>39.92</v>
+      </c>
+      <c r="H71">
+        <v>516</v>
+      </c>
+      <c r="I71" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B72">
+        <v>1</v>
+      </c>
+      <c r="C72" t="s">
+        <v>5</v>
+      </c>
+      <c r="D72">
+        <v>708.2</v>
+      </c>
+      <c r="E72">
+        <v>0.747</v>
+      </c>
+      <c r="F72">
+        <v>238</v>
+      </c>
+      <c r="G72">
+        <v>40.82</v>
+      </c>
+      <c r="H72">
+        <v>529</v>
+      </c>
+      <c r="I72" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B73">
+        <v>1</v>
+      </c>
+      <c r="C73" t="s">
+        <v>5</v>
+      </c>
+      <c r="D73">
+        <v>696.6</v>
+      </c>
+      <c r="E73">
+        <v>0.74929999999999997</v>
+      </c>
+      <c r="F73">
+        <v>238</v>
+      </c>
+      <c r="G73">
+        <v>40.28</v>
+      </c>
+      <c r="H73">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B74">
+        <v>1</v>
+      </c>
+      <c r="C74" t="s">
+        <v>5</v>
+      </c>
+      <c r="D74">
+        <v>760</v>
+      </c>
+      <c r="E74">
+        <v>0.7379</v>
+      </c>
+      <c r="F74">
+        <v>238</v>
+      </c>
+      <c r="G74">
+        <v>43.3</v>
+      </c>
+      <c r="H74">
+        <v>561</v>
+      </c>
+      <c r="I74" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B76">
+        <v>1</v>
+      </c>
+      <c r="C76" t="s">
+        <v>5</v>
+      </c>
+      <c r="D76">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B77">
+        <v>1</v>
+      </c>
+      <c r="C77" t="s">
+        <v>5</v>
+      </c>
+      <c r="D77">
+        <v>716.2</v>
+      </c>
+      <c r="E77">
+        <v>0.74839999999999995</v>
+      </c>
+      <c r="F77">
+        <v>238</v>
+      </c>
+      <c r="G77">
+        <v>41.482700000000001</v>
+      </c>
+      <c r="H77">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B78">
+        <v>1</v>
+      </c>
+      <c r="C78" t="s">
+        <v>5</v>
+      </c>
+      <c r="D78">
+        <v>653</v>
+      </c>
+      <c r="E78">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="F78">
+        <v>238</v>
+      </c>
+      <c r="G78">
+        <v>39.1</v>
+      </c>
+      <c r="H78">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B79">
+        <v>1</v>
+      </c>
+      <c r="C79" t="s">
+        <v>5</v>
+      </c>
+      <c r="D79">
+        <v>629.4</v>
+      </c>
+      <c r="E79">
+        <v>0.8246</v>
+      </c>
+      <c r="F79">
+        <v>238</v>
+      </c>
+      <c r="G79">
+        <v>40.06</v>
+      </c>
+      <c r="H79">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B80">
+        <v>1</v>
+      </c>
+      <c r="C80" t="s">
+        <v>10</v>
+      </c>
+      <c r="D80">
+        <v>757</v>
+      </c>
+      <c r="E80">
+        <v>0.74239999999999995</v>
+      </c>
+      <c r="F80">
+        <v>238</v>
+      </c>
+      <c r="G80">
+        <v>43.513500000000001</v>
+      </c>
+      <c r="H80">
+        <v>562</v>
+      </c>
+      <c r="I80" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B81">
+        <v>1</v>
+      </c>
+      <c r="C81" t="s">
+        <v>10</v>
+      </c>
+      <c r="D81">
+        <v>729</v>
+      </c>
+      <c r="E81">
+        <v>0.746</v>
+      </c>
+      <c r="F81">
+        <v>238</v>
+      </c>
+      <c r="G81">
+        <v>42</v>
+      </c>
+      <c r="H81">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B82">
+        <v>1</v>
+      </c>
+      <c r="C82" t="s">
+        <v>10</v>
+      </c>
+      <c r="D82">
+        <v>690</v>
+      </c>
+      <c r="E82">
+        <v>0.75219999999999998</v>
+      </c>
+      <c r="F82">
+        <v>238</v>
+      </c>
+      <c r="G82">
+        <v>40.299999999999997</v>
+      </c>
+      <c r="H82">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B83">
+        <v>1</v>
+      </c>
+      <c r="C83" t="s">
+        <v>10</v>
+      </c>
+      <c r="D83">
+        <v>675</v>
+      </c>
+      <c r="E83">
+        <v>0.74860000000000004</v>
+      </c>
+      <c r="F83">
+        <v>238</v>
+      </c>
+      <c r="G83">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="H83">
+        <v>506</v>
+      </c>
+      <c r="I83" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B84">
+        <v>1</v>
+      </c>
+      <c r="C84" t="s">
+        <v>5</v>
+      </c>
+      <c r="D84">
+        <v>728</v>
+      </c>
+      <c r="E84">
+        <v>0.74239999999999995</v>
+      </c>
+      <c r="F84">
+        <v>238</v>
+      </c>
+      <c r="G84">
+        <v>41.77</v>
+      </c>
+      <c r="H84">
+        <v>541</v>
+      </c>
+      <c r="I84" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B85">
+        <v>1</v>
+      </c>
+      <c r="C85" t="s">
+        <v>5</v>
+      </c>
+      <c r="D85">
+        <v>727.5</v>
+      </c>
+      <c r="E85">
+        <v>0.74229999999999996</v>
+      </c>
+      <c r="F85">
+        <v>238</v>
+      </c>
+      <c r="G85">
+        <v>42.84</v>
+      </c>
+      <c r="H85">
+        <v>540</v>
+      </c>
+      <c r="I85" t="s">
+        <v>164</v>
+      </c>
+      <c r="J85" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B86">
+        <v>1</v>
+      </c>
+      <c r="C86" t="s">
+        <v>5</v>
+      </c>
+      <c r="D86">
+        <v>727.2</v>
+      </c>
+      <c r="E86">
+        <v>0.7329</v>
+      </c>
+      <c r="F86">
+        <v>238</v>
+      </c>
+      <c r="G86">
+        <v>42.8</v>
+      </c>
+      <c r="H86">
+        <v>533</v>
+      </c>
+      <c r="I86" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I87" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B88">
+        <v>2</v>
+      </c>
+      <c r="C88" t="s">
+        <v>5</v>
+      </c>
+      <c r="D88">
+        <v>739.2</v>
+      </c>
+      <c r="E88">
+        <v>1.5246</v>
+      </c>
+      <c r="F88">
+        <v>478</v>
+      </c>
+      <c r="G88">
+        <v>112.05</v>
+      </c>
+      <c r="H88">
+        <v>1127</v>
+      </c>
+      <c r="I88" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D89">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B91">
+        <v>1</v>
+      </c>
+      <c r="C91" t="s">
+        <v>5</v>
+      </c>
+      <c r="D91">
+        <v>910.25</v>
+      </c>
+      <c r="E91">
+        <v>0.71960000000000002</v>
+      </c>
+      <c r="F91">
+        <v>238</v>
+      </c>
+      <c r="G91">
+        <v>65.25</v>
+      </c>
+      <c r="H91">
+        <v>655</v>
+      </c>
+      <c r="I91" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B92">
+        <v>1</v>
+      </c>
+      <c r="C92" t="s">
+        <v>5</v>
+      </c>
+      <c r="D92">
+        <v>966</v>
+      </c>
+      <c r="E92">
+        <v>0.66049999999999998</v>
+      </c>
+      <c r="F92">
+        <v>238</v>
+      </c>
+      <c r="G92">
+        <v>63.67</v>
+      </c>
+      <c r="H92">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B93">
+        <v>1</v>
+      </c>
+      <c r="C93" t="s">
+        <v>5</v>
+      </c>
+      <c r="D93">
+        <v>1003.5</v>
+      </c>
+      <c r="E93">
+        <v>0.65169999999999995</v>
+      </c>
+      <c r="F93">
+        <v>238</v>
+      </c>
+      <c r="G93">
+        <v>65.3</v>
+      </c>
+      <c r="H93">
+        <v>654</v>
+      </c>
+      <c r="I93" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B94">
+        <v>1</v>
+      </c>
+      <c r="C94" t="s">
+        <v>5</v>
+      </c>
+      <c r="D94">
+        <v>964.2</v>
+      </c>
+      <c r="E94">
+        <v>0.65439999999999998</v>
+      </c>
+      <c r="F94">
+        <v>238</v>
+      </c>
+      <c r="G94">
+        <v>63</v>
+      </c>
+      <c r="H94">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B95">
+        <v>1</v>
+      </c>
+      <c r="C95" t="s">
+        <v>5</v>
+      </c>
+      <c r="D95">
+        <v>991</v>
+      </c>
+      <c r="E95">
+        <v>0.64939999999999998</v>
+      </c>
+      <c r="F95">
+        <v>238</v>
+      </c>
+      <c r="G95">
+        <v>65</v>
+      </c>
+      <c r="H95">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B96">
+        <v>1</v>
+      </c>
+      <c r="C96" t="s">
+        <v>10</v>
+      </c>
+      <c r="D96">
+        <v>1199</v>
+      </c>
+      <c r="E96">
+        <v>0.61870000000000003</v>
+      </c>
+      <c r="F96">
+        <v>238</v>
+      </c>
+      <c r="G96">
+        <v>73.819999999999993</v>
+      </c>
+      <c r="H96">
+        <v>742</v>
+      </c>
+      <c r="I96" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B97">
+        <v>1</v>
+      </c>
+      <c r="C97" t="s">
+        <v>10</v>
+      </c>
+      <c r="D97">
+        <v>1017</v>
+      </c>
+      <c r="E97">
+        <v>0.65339999999999998</v>
+      </c>
+      <c r="F97">
+        <v>238</v>
+      </c>
+      <c r="G97">
+        <v>66.16</v>
+      </c>
+      <c r="H97">
+        <v>665</v>
+      </c>
+      <c r="I97" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B98">
+        <v>1</v>
+      </c>
+      <c r="C98" t="s">
+        <v>10</v>
+      </c>
+      <c r="D98">
+        <v>954</v>
+      </c>
+      <c r="E98">
+        <v>0.66459999999999997</v>
+      </c>
+      <c r="F98">
+        <v>238</v>
+      </c>
+      <c r="G98">
+        <v>63</v>
+      </c>
+      <c r="H98">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B99">
+        <v>1</v>
+      </c>
+      <c r="C99" t="s">
+        <v>10</v>
+      </c>
+      <c r="D99">
+        <v>991.67</v>
+      </c>
+      <c r="E99">
+        <v>0.65749999999999997</v>
+      </c>
+      <c r="F99">
+        <v>238</v>
+      </c>
+      <c r="G99">
+        <v>64.8</v>
+      </c>
+      <c r="H99">
+        <v>652</v>
+      </c>
+      <c r="I99" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B100">
+        <v>1</v>
+      </c>
+      <c r="C100" t="s">
+        <v>5</v>
+      </c>
+      <c r="D100">
+        <v>991.75</v>
+      </c>
+      <c r="E100">
+        <v>0.65239999999999998</v>
+      </c>
+      <c r="F100">
+        <v>238</v>
+      </c>
+      <c r="G100">
+        <v>65.459999999999994</v>
+      </c>
+      <c r="H100">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B101">
+        <v>1</v>
+      </c>
+      <c r="C101" t="s">
+        <v>5</v>
+      </c>
+      <c r="D101">
+        <v>927.6</v>
+      </c>
+      <c r="E101">
+        <v>0.71579999999999999</v>
+      </c>
+      <c r="F101">
+        <v>238</v>
+      </c>
+      <c r="G101">
+        <v>66.150000000000006</v>
+      </c>
+      <c r="H101">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B102">
+        <v>1</v>
+      </c>
+      <c r="C102" t="s">
+        <v>5</v>
+      </c>
+      <c r="D102">
+        <v>951.7</v>
+      </c>
+      <c r="E102">
+        <v>0.71030000000000004</v>
+      </c>
+      <c r="F102">
+        <v>238</v>
+      </c>
+      <c r="G102">
+        <v>67.5</v>
+      </c>
+      <c r="H102">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B103">
+        <v>1</v>
+      </c>
+      <c r="C103" t="s">
+        <v>5</v>
+      </c>
+      <c r="D103">
+        <v>921.5</v>
+      </c>
+      <c r="E103">
+        <v>0.71730000000000005</v>
+      </c>
+      <c r="F103">
+        <v>238</v>
+      </c>
+      <c r="G103">
+        <v>65.8</v>
+      </c>
+      <c r="H103">
+        <v>661</v>
+      </c>
+      <c r="I103" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B104">
+        <v>1</v>
+      </c>
+      <c r="C104" t="s">
+        <v>5</v>
+      </c>
+      <c r="D104">
+        <v>1073.7</v>
+      </c>
+      <c r="E104">
+        <v>0.62680000000000002</v>
+      </c>
+      <c r="F104">
+        <v>238</v>
+      </c>
+      <c r="G104">
+        <v>68.7</v>
+      </c>
+      <c r="H104">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B105">
+        <v>1</v>
+      </c>
+      <c r="C105" t="s">
+        <v>5</v>
+      </c>
+      <c r="D105">
+        <v>1000.05</v>
+      </c>
+      <c r="E105">
+        <v>0.7</v>
+      </c>
+      <c r="F105">
+        <v>238</v>
+      </c>
+      <c r="G105">
+        <v>70</v>
+      </c>
+      <c r="H105">
+        <v>700</v>
+      </c>
+      <c r="I105" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="3"/>
+    </row>
+    <row r="107" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="3"/>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A109" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B109">
+        <v>3</v>
+      </c>
+      <c r="C109" t="s">
+        <v>5</v>
+      </c>
+      <c r="D109">
+        <v>2306</v>
+      </c>
+      <c r="E109">
+        <v>1.6829000000000001</v>
+      </c>
+      <c r="F109">
+        <v>718</v>
+      </c>
+      <c r="G109">
+        <v>301.2</v>
+      </c>
+      <c r="H109">
+        <v>3881</v>
+      </c>
+      <c r="I109" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A110" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B110">
+        <v>3</v>
+      </c>
+      <c r="C110" t="s">
+        <v>5</v>
+      </c>
+      <c r="D110">
+        <v>2305</v>
+      </c>
+      <c r="E110">
+        <v>1.6835</v>
+      </c>
+      <c r="F110">
+        <v>718</v>
+      </c>
+      <c r="G110">
+        <v>301.5</v>
+      </c>
+      <c r="H110">
+        <v>3881</v>
+      </c>
+      <c r="I110" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A111" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B111">
+        <v>3</v>
+      </c>
+      <c r="C111" t="s">
+        <v>5</v>
+      </c>
+      <c r="D111">
+        <v>2299</v>
+      </c>
+      <c r="E111">
+        <v>1.6828000000000001</v>
+      </c>
+      <c r="F111">
+        <v>718</v>
+      </c>
+      <c r="G111">
+        <v>300.89</v>
+      </c>
+      <c r="H111">
+        <v>3870</v>
+      </c>
+      <c r="I111" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A112" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B112">
+        <v>3</v>
+      </c>
+      <c r="C112" t="s">
+        <v>10</v>
+      </c>
+      <c r="D112">
+        <v>2196.4</v>
+      </c>
+      <c r="E112">
+        <v>1.7464999999999999</v>
+      </c>
+      <c r="F112">
+        <v>718</v>
+      </c>
+      <c r="G112">
+        <v>298.8</v>
+      </c>
+      <c r="H112">
+        <v>3836</v>
+      </c>
+      <c r="I112" t="s">
+        <v>198</v>
+      </c>
+      <c r="J112" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A113" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B113">
+        <v>3</v>
+      </c>
+      <c r="C113" t="s">
+        <v>10</v>
+      </c>
+      <c r="D113">
+        <v>2127.1999999999998</v>
+      </c>
+      <c r="E113">
+        <v>1.7713000000000001</v>
+      </c>
+      <c r="F113">
+        <v>718</v>
+      </c>
+      <c r="G113">
+        <v>292.8</v>
+      </c>
+      <c r="H113">
+        <v>3768</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A114" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B114">
+        <v>3</v>
+      </c>
+      <c r="C114" t="s">
+        <v>10</v>
+      </c>
+      <c r="D114">
+        <v>2195.8000000000002</v>
+      </c>
+      <c r="E114">
+        <v>1.7151000000000001</v>
+      </c>
+      <c r="F114">
+        <v>718</v>
+      </c>
+      <c r="G114">
+        <v>293.39999999999998</v>
+      </c>
+      <c r="H114">
+        <v>3766</v>
+      </c>
+      <c r="I114" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A115" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B115">
+        <v>3</v>
+      </c>
+      <c r="C115" t="s">
+        <v>5</v>
+      </c>
+      <c r="D115">
+        <v>2340.6</v>
+      </c>
+      <c r="E115">
+        <v>1.6675</v>
+      </c>
+      <c r="F115">
+        <v>718</v>
+      </c>
+      <c r="G115">
+        <v>304</v>
+      </c>
+      <c r="H115">
+        <v>3903</v>
+      </c>
+      <c r="I115" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A116" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B116">
+        <v>3</v>
+      </c>
+      <c r="C116" t="s">
+        <v>5</v>
+      </c>
+      <c r="D116">
+        <v>2229.6999999999998</v>
+      </c>
+      <c r="E116">
+        <v>1.7397</v>
+      </c>
+      <c r="F116">
+        <v>718</v>
+      </c>
+      <c r="G116">
+        <v>300.45999999999998</v>
+      </c>
+      <c r="H116">
+        <v>3879</v>
+      </c>
+      <c r="I116" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A117" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B117">
+        <v>3</v>
+      </c>
+      <c r="C117" t="s">
+        <v>5</v>
+      </c>
+      <c r="D117">
+        <v>2250.1</v>
+      </c>
+      <c r="E117">
+        <v>1.7310000000000001</v>
+      </c>
+      <c r="F117">
+        <v>718</v>
+      </c>
+      <c r="G117">
+        <v>302.5</v>
+      </c>
+      <c r="H117">
+        <v>3895</v>
+      </c>
+      <c r="I117" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A118" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A120" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B120">
+        <v>1</v>
+      </c>
+      <c r="C120" t="s">
+        <v>5</v>
+      </c>
+      <c r="D120">
+        <v>1580.89</v>
+      </c>
+      <c r="E120">
+        <v>0.62309999999999999</v>
+      </c>
+      <c r="F120">
+        <v>238</v>
+      </c>
+      <c r="G120">
+        <v>76.8</v>
+      </c>
+      <c r="H120">
+        <v>985</v>
+      </c>
+      <c r="I120" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A121" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B121">
+        <v>1</v>
+      </c>
+      <c r="C121" t="s">
+        <v>5</v>
+      </c>
+      <c r="D121">
+        <v>2099.66</v>
+      </c>
+      <c r="E121">
+        <v>0.54679999999999995</v>
+      </c>
+      <c r="F121">
+        <v>238</v>
+      </c>
+      <c r="G121">
+        <v>89.4</v>
+      </c>
+      <c r="H121">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A122" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B122">
+        <v>1</v>
+      </c>
+      <c r="C122" t="s">
+        <v>5</v>
+      </c>
+      <c r="D122">
+        <v>2106.9</v>
+      </c>
+      <c r="E122">
+        <v>0.54390000000000005</v>
+      </c>
+      <c r="F122">
+        <v>238</v>
+      </c>
+      <c r="G122">
+        <v>90.23</v>
+      </c>
+      <c r="H122">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A123" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B123">
+        <v>1</v>
+      </c>
+      <c r="C123" t="s">
+        <v>5</v>
+      </c>
+      <c r="D123">
+        <v>1784.2</v>
+      </c>
+      <c r="E123">
+        <v>0.62770000000000004</v>
+      </c>
+      <c r="F123">
+        <v>238</v>
+      </c>
+      <c r="G123">
+        <v>87.3</v>
+      </c>
+      <c r="H123">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A124" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B124">
+        <v>1</v>
+      </c>
+      <c r="C124" t="s">
+        <v>5</v>
+      </c>
+      <c r="D124">
+        <v>2082.1999999999998</v>
+      </c>
+      <c r="E124">
+        <v>0.54749999999999999</v>
+      </c>
+      <c r="F124">
+        <v>238</v>
+      </c>
+      <c r="G124">
+        <v>89.6</v>
+      </c>
+      <c r="H124">
+        <v>1140</v>
+      </c>
+      <c r="I124" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A125" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B125">
+        <v>1</v>
+      </c>
+      <c r="C125" t="s">
+        <v>10</v>
+      </c>
+      <c r="D125">
+        <v>2128.4</v>
+      </c>
+      <c r="E125">
+        <v>0.53979999999999995</v>
+      </c>
+      <c r="F125">
+        <v>238</v>
+      </c>
+      <c r="G125">
+        <v>89.66</v>
+      </c>
+      <c r="H125">
+        <v>1149</v>
+      </c>
+      <c r="I125" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A126" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="B126">
+        <v>1</v>
+      </c>
+      <c r="C126" t="s">
+        <v>10</v>
+      </c>
+      <c r="D126">
+        <v>1740.86</v>
+      </c>
+      <c r="E126">
+        <v>0.63470000000000004</v>
+      </c>
+      <c r="F126">
+        <v>238</v>
+      </c>
+      <c r="G126">
+        <v>85.6</v>
+      </c>
+      <c r="H126">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A127" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B127">
+        <v>1</v>
+      </c>
+      <c r="C127" t="s">
+        <v>10</v>
+      </c>
+      <c r="D127">
+        <v>1734.32</v>
+      </c>
+      <c r="E127">
+        <v>0.63370000000000004</v>
+      </c>
+      <c r="F127">
+        <v>238</v>
+      </c>
+      <c r="G127">
+        <v>85.87</v>
+      </c>
+      <c r="H127">
+        <v>1099</v>
+      </c>
+      <c r="I127" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A128" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B128">
+        <v>1</v>
+      </c>
+      <c r="C128" t="s">
+        <v>10</v>
+      </c>
+      <c r="D128">
+        <v>2021.78</v>
+      </c>
+      <c r="E128">
+        <v>0.55349999999999999</v>
+      </c>
+      <c r="F128">
+        <v>238</v>
+      </c>
+      <c r="G128">
+        <v>87.36</v>
+      </c>
+      <c r="H128">
+        <v>1119</v>
+      </c>
+      <c r="I128" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A129" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="B129">
+        <v>1</v>
+      </c>
+      <c r="C129" t="s">
+        <v>10</v>
+      </c>
+      <c r="D129">
+        <v>1927.2</v>
+      </c>
+      <c r="E129">
+        <v>0.56710000000000005</v>
+      </c>
+      <c r="F129">
+        <v>238</v>
+      </c>
+      <c r="G129">
+        <v>84.78</v>
+      </c>
+      <c r="H129">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A130" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="B130">
+        <v>1</v>
+      </c>
+      <c r="C130" t="s">
+        <v>5</v>
+      </c>
+      <c r="D130">
+        <v>1900.3</v>
+      </c>
+      <c r="E130">
+        <v>0.61519999999999997</v>
+      </c>
+      <c r="F130">
+        <v>238</v>
+      </c>
+      <c r="G130">
+        <v>90.34</v>
+      </c>
+      <c r="H130">
+        <v>1169</v>
+      </c>
+      <c r="I130" t="s">
+        <v>228</v>
+      </c>
+      <c r="J130" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A131" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="B131">
+        <v>1</v>
+      </c>
+      <c r="C131" t="s">
+        <v>5</v>
+      </c>
+      <c r="D131">
+        <v>2074.3000000000002</v>
+      </c>
+      <c r="E131">
+        <v>0.54759999999999998</v>
+      </c>
+      <c r="F131">
+        <v>238</v>
+      </c>
+      <c r="G131">
+        <v>88.74</v>
+      </c>
+      <c r="H131">
+        <v>1136</v>
+      </c>
+      <c r="I131" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A132" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="B132">
+        <v>1</v>
+      </c>
+      <c r="C132" t="s">
+        <v>5</v>
+      </c>
+      <c r="D132">
+        <v>1984.2</v>
+      </c>
+      <c r="E132">
+        <v>0.57399999999999995</v>
+      </c>
+      <c r="F132">
+        <v>238</v>
+      </c>
+      <c r="G132">
+        <v>88.5</v>
+      </c>
+      <c r="H132">
+        <v>1139</v>
+      </c>
+      <c r="I132" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A133" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="B133">
+        <v>1</v>
+      </c>
+      <c r="C133" t="s">
+        <v>5</v>
+      </c>
+      <c r="D133">
+        <v>1981</v>
+      </c>
+      <c r="E133">
+        <v>0.56130000000000002</v>
+      </c>
+      <c r="F133">
+        <v>238</v>
+      </c>
+      <c r="G133">
+        <v>86.15</v>
+      </c>
+      <c r="H133">
+        <v>1112</v>
+      </c>
+      <c r="I133" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A134" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="B134">
+        <v>1</v>
+      </c>
+      <c r="C134" t="s">
+        <v>5</v>
+      </c>
+      <c r="D134">
+        <v>2079.3000000000002</v>
+      </c>
+      <c r="E134">
+        <v>0.54779999999999995</v>
+      </c>
+      <c r="F134">
+        <v>238</v>
+      </c>
+      <c r="G134">
+        <v>89.14</v>
+      </c>
+      <c r="H134">
+        <v>1139</v>
+      </c>
+      <c r="I134" t="s">
+        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update with guinardian 5ml vert runs
</commit_message>
<xml_diff>
--- a/Development/IFCB_vehicles/VehicleLabExperimentFiles.xlsx
+++ b/Development/IFCB_vehicles/VehicleLabExperimentFiles.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="5085" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="5085" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="VvsHdiffVol_nogood" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="9um_beads" sheetId="2" r:id="rId2"/>
+    <sheet name="Guinardia" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="243">
   <si>
     <t>Filename</t>
   </si>
@@ -730,6 +731,30 @@
   </si>
   <si>
     <t>all look good</t>
+  </si>
+  <si>
+    <t>D20151112T164628</t>
+  </si>
+  <si>
+    <t>2nd syringe from gui, still some beads, first sucked 5ml sample then run ~1ml</t>
+  </si>
+  <si>
+    <t>use all triggers</t>
+  </si>
+  <si>
+    <t>D20151112T170931</t>
+  </si>
+  <si>
+    <t>still some beads</t>
+  </si>
+  <si>
+    <t>D20151112T173151</t>
+  </si>
+  <si>
+    <t>D20151112T175410</t>
+  </si>
+  <si>
+    <t>D20151112T181728</t>
   </si>
 </sst>
 </file>
@@ -1369,9 +1394,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L134"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I135" sqref="I135"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4919,4 +4944,220 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I6" sqref="I6:J6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>373.43599999999998</v>
+      </c>
+      <c r="E2">
+        <v>4.1212</v>
+      </c>
+      <c r="F2">
+        <v>1198</v>
+      </c>
+      <c r="G2">
+        <v>193.9</v>
+      </c>
+      <c r="H2">
+        <v>1539</v>
+      </c>
+      <c r="I2" t="s">
+        <v>237</v>
+      </c>
+      <c r="J2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>238</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>492</v>
+      </c>
+      <c r="E3">
+        <v>3.9977</v>
+      </c>
+      <c r="F3">
+        <v>1198</v>
+      </c>
+      <c r="G3">
+        <v>224.2</v>
+      </c>
+      <c r="H3">
+        <v>1967</v>
+      </c>
+      <c r="I3" t="s">
+        <v>237</v>
+      </c>
+      <c r="J3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>240</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>629.58000000000004</v>
+      </c>
+      <c r="E4">
+        <v>3.8645</v>
+      </c>
+      <c r="F4">
+        <v>1198</v>
+      </c>
+      <c r="G4">
+        <v>262.5</v>
+      </c>
+      <c r="H4">
+        <v>2433</v>
+      </c>
+      <c r="I4" t="s">
+        <v>237</v>
+      </c>
+      <c r="J4" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>241</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>742.7</v>
+      </c>
+      <c r="E5">
+        <v>3.7456999999999998</v>
+      </c>
+      <c r="F5">
+        <v>1198</v>
+      </c>
+      <c r="G5">
+        <v>284</v>
+      </c>
+      <c r="H5">
+        <v>2782</v>
+      </c>
+      <c r="I5" t="s">
+        <v>237</v>
+      </c>
+      <c r="J5" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>242</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>790.7</v>
+      </c>
+      <c r="E6">
+        <v>3.7143999999999999</v>
+      </c>
+      <c r="F6">
+        <v>1198</v>
+      </c>
+      <c r="G6">
+        <v>291.2</v>
+      </c>
+      <c r="H6">
+        <v>2937</v>
+      </c>
+      <c r="I6" t="s">
+        <v>237</v>
+      </c>
+      <c r="J6" t="s">
+        <v>239</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated gui runs with all 5ml and 1ml runs
</commit_message>
<xml_diff>
--- a/Development/IFCB_vehicles/VehicleLabExperimentFiles.xlsx
+++ b/Development/IFCB_vehicles/VehicleLabExperimentFiles.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\ifcb-analysis\Development\IFCB_vehicles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\from_Samwise\ifcb-analysis\Development\IFCB_vehicles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="285">
   <si>
     <t>Filename</t>
   </si>
@@ -755,6 +755,132 @@
   </si>
   <si>
     <t>D20151112T181728</t>
+  </si>
+  <si>
+    <t>D20151112T184118</t>
+  </si>
+  <si>
+    <t>looked at all rois, no bubble</t>
+  </si>
+  <si>
+    <t>D20151112T191233</t>
+  </si>
+  <si>
+    <t>D20151112T193452</t>
+  </si>
+  <si>
+    <t>D20151112T195712</t>
+  </si>
+  <si>
+    <t>went to check flask and a decent kink where intake tubing meets Si tubing of other part, try to adjust so no kink, could that have been breaking up some of the cells when turning?</t>
+  </si>
+  <si>
+    <t>D20151112T201931</t>
+  </si>
+  <si>
+    <t>don't include in analysis</t>
+  </si>
+  <si>
+    <t>&gt;150CellConc</t>
+  </si>
+  <si>
+    <t>D20151112T204151</t>
+  </si>
+  <si>
+    <t>Count &gt;150</t>
+  </si>
+  <si>
+    <t>D20151112T210954</t>
+  </si>
+  <si>
+    <t>D20151112T213214</t>
+  </si>
+  <si>
+    <t>D20151112T215433</t>
+  </si>
+  <si>
+    <t>D20151112T221653</t>
+  </si>
+  <si>
+    <t>SWITCH TO 1ML</t>
+  </si>
+  <si>
+    <t>D20151112T224220</t>
+  </si>
+  <si>
+    <t>not many long cells at all, more med now, stir bar going crazy some, maybe breaking more</t>
+  </si>
+  <si>
+    <t>D20151112T224924</t>
+  </si>
+  <si>
+    <t>D20151112T225523</t>
+  </si>
+  <si>
+    <t>D20151112T230123</t>
+  </si>
+  <si>
+    <t>D20151112T230723</t>
+  </si>
+  <si>
+    <t>D20151112T231706</t>
+  </si>
+  <si>
+    <t>still some beads, a few large pieces of junk</t>
+  </si>
+  <si>
+    <t>stir bar has been going crazy more</t>
+  </si>
+  <si>
+    <t>D20151112T232306</t>
+  </si>
+  <si>
+    <t>D20151112T232906</t>
+  </si>
+  <si>
+    <t>D20151112T233506</t>
+  </si>
+  <si>
+    <t>D20151112T234106</t>
+  </si>
+  <si>
+    <t>D20151112T235221</t>
+  </si>
+  <si>
+    <t>D20151112T235821</t>
+  </si>
+  <si>
+    <t>getting to be lots of junk</t>
+  </si>
+  <si>
+    <t>x&gt;150 &amp; y&lt;100 conc</t>
+  </si>
+  <si>
+    <t>count &gt;150 &amp; &lt;100</t>
+  </si>
+  <si>
+    <t>D20151113T000421</t>
+  </si>
+  <si>
+    <t>MANY MISSED ROIS, BAD CORE POS, MUST BE BUBBLE OR JUNK STUCK, NO SEE BUBBLE</t>
+  </si>
+  <si>
+    <t>D20151113T001020</t>
+  </si>
+  <si>
+    <t>3 or 4 microbubbles</t>
+  </si>
+  <si>
+    <t>2nd isin better gets rid of some junk and bubbles</t>
+  </si>
+  <si>
+    <t>D20151113T001620</t>
+  </si>
+  <si>
+    <t>D20151113T003006</t>
+  </si>
+  <si>
+    <t>lots of junkat this point</t>
   </si>
 </sst>
 </file>
@@ -4948,11 +5074,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I6" sqref="I6:J6"/>
+      <selection pane="bottomLeft" activeCell="D33" sqref="D33:E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4960,12 +5086,13 @@
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="17.42578125" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4979,121 +5106,160 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="N1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="B2">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2">
+      <c r="B2" s="2">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2">
         <v>373.43599999999998</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
+        <v>220.57</v>
+      </c>
+      <c r="G2" s="2">
+        <v>909</v>
+      </c>
+      <c r="I2" s="2">
         <v>4.1212</v>
       </c>
-      <c r="F2">
+      <c r="J2" s="2">
         <v>1198</v>
       </c>
-      <c r="G2">
+      <c r="K2" s="2">
         <v>193.9</v>
       </c>
-      <c r="H2">
+      <c r="L2" s="2">
         <v>1539</v>
       </c>
-      <c r="I2" t="s">
+      <c r="M2" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="J2" t="s">
+      <c r="N2" s="2" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>238</v>
-      </c>
-      <c r="B3">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3">
+      <c r="P2" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B3" s="2">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2">
         <v>492</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
+        <v>279.39999999999998</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1117</v>
+      </c>
+      <c r="I3" s="2">
         <v>3.9977</v>
       </c>
-      <c r="F3">
+      <c r="J3" s="2">
         <v>1198</v>
       </c>
-      <c r="G3">
+      <c r="K3" s="2">
         <v>224.2</v>
       </c>
-      <c r="H3">
+      <c r="L3" s="2">
         <v>1967</v>
       </c>
-      <c r="I3" t="s">
+      <c r="M3" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="J3" t="s">
+      <c r="N3" s="2" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="P3" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B4">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4">
+      <c r="B4" s="2">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2">
         <v>629.58000000000004</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
+        <v>316.47000000000003</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1223</v>
+      </c>
+      <c r="I4" s="2">
         <v>3.8645</v>
       </c>
-      <c r="F4">
+      <c r="J4" s="2">
         <v>1198</v>
       </c>
-      <c r="G4">
+      <c r="K4" s="2">
         <v>262.5</v>
       </c>
-      <c r="H4">
+      <c r="L4" s="2">
         <v>2433</v>
       </c>
-      <c r="I4" t="s">
+      <c r="M4" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="J4" t="s">
+      <c r="N4" s="2" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="P4" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>241</v>
       </c>
@@ -5107,25 +5273,31 @@
         <v>742.7</v>
       </c>
       <c r="E5">
+        <v>427.7</v>
+      </c>
+      <c r="G5">
+        <v>1602</v>
+      </c>
+      <c r="I5">
         <v>3.7456999999999998</v>
       </c>
-      <c r="F5">
+      <c r="J5">
         <v>1198</v>
       </c>
-      <c r="G5">
+      <c r="K5">
         <v>284</v>
       </c>
-      <c r="H5">
+      <c r="L5">
         <v>2782</v>
       </c>
-      <c r="I5" t="s">
+      <c r="M5" t="s">
         <v>237</v>
       </c>
-      <c r="J5" t="s">
+      <c r="N5" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>242</v>
       </c>
@@ -5139,25 +5311,1061 @@
         <v>790.7</v>
       </c>
       <c r="E6">
+        <v>503.2</v>
+      </c>
+      <c r="G6">
+        <v>1869</v>
+      </c>
+      <c r="I6">
         <v>3.7143999999999999</v>
       </c>
-      <c r="F6">
+      <c r="J6">
         <v>1198</v>
       </c>
-      <c r="G6">
+      <c r="K6">
         <v>291.2</v>
       </c>
-      <c r="H6">
+      <c r="L6">
         <v>2937</v>
       </c>
-      <c r="I6" t="s">
+      <c r="M6" t="s">
         <v>237</v>
       </c>
-      <c r="J6" t="s">
+      <c r="N6" t="s">
         <v>239</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>243</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>757.3</v>
+      </c>
+      <c r="E7">
+        <v>473.1</v>
+      </c>
+      <c r="G7">
+        <v>1791</v>
+      </c>
+      <c r="I7">
+        <v>3.7858000000000001</v>
+      </c>
+      <c r="J7">
+        <v>1198</v>
+      </c>
+      <c r="K7">
+        <v>274.89999999999998</v>
+      </c>
+      <c r="L7">
+        <v>2867</v>
+      </c>
+      <c r="M7" t="s">
+        <v>237</v>
+      </c>
+      <c r="N7" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>245</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>673.8</v>
+      </c>
+      <c r="E8">
+        <v>387</v>
+      </c>
+      <c r="G8">
+        <v>1503</v>
+      </c>
+      <c r="I8">
+        <v>3.8837000000000002</v>
+      </c>
+      <c r="J8">
+        <v>1198</v>
+      </c>
+      <c r="K8">
+        <v>250.4</v>
+      </c>
+      <c r="L8">
+        <v>2617</v>
+      </c>
+      <c r="M8" t="s">
+        <v>237</v>
+      </c>
+      <c r="N8" t="s">
+        <v>239</v>
+      </c>
+      <c r="O8" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>246</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>645</v>
+      </c>
+      <c r="E9">
+        <v>378.84</v>
+      </c>
+      <c r="G9">
+        <v>1515</v>
+      </c>
+      <c r="I9">
+        <v>3.99</v>
+      </c>
+      <c r="J9">
+        <v>1198</v>
+      </c>
+      <c r="K9">
+        <v>237.19</v>
+      </c>
+      <c r="L9">
+        <v>2580</v>
+      </c>
+      <c r="M9" t="s">
+        <v>237</v>
+      </c>
+      <c r="N9" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>247</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>631</v>
+      </c>
+      <c r="E10">
+        <v>383</v>
+      </c>
+      <c r="G10">
+        <v>1515</v>
+      </c>
+      <c r="I10">
+        <v>3.9556</v>
+      </c>
+      <c r="J10">
+        <v>1198</v>
+      </c>
+      <c r="K10">
+        <v>233.56800000000001</v>
+      </c>
+      <c r="L10">
+        <v>2496</v>
+      </c>
+      <c r="M10" t="s">
+        <v>237</v>
+      </c>
+      <c r="N10" t="s">
+        <v>239</v>
+      </c>
+      <c r="O10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>249</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>678.8</v>
+      </c>
+      <c r="E11">
+        <v>416.15</v>
+      </c>
+      <c r="G11">
+        <v>1616</v>
+      </c>
+      <c r="I11">
+        <v>3.8832</v>
+      </c>
+      <c r="J11">
+        <v>1198</v>
+      </c>
+      <c r="K11">
+        <v>250</v>
+      </c>
+      <c r="L11">
+        <v>2636</v>
+      </c>
+      <c r="M11" t="s">
+        <v>248</v>
+      </c>
+      <c r="N11" t="s">
+        <v>237</v>
+      </c>
+      <c r="O11" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>252</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <v>644.36</v>
+      </c>
+      <c r="E12">
+        <v>398.54</v>
+      </c>
+      <c r="G12">
+        <v>1584</v>
+      </c>
+      <c r="I12">
+        <v>3.9744999999999999</v>
+      </c>
+      <c r="J12">
+        <v>1198</v>
+      </c>
+      <c r="K12">
+        <v>244.1</v>
+      </c>
+      <c r="L12">
+        <v>2561</v>
+      </c>
+      <c r="M12" t="s">
+        <v>237</v>
+      </c>
+      <c r="N12" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>254</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>774.85</v>
+      </c>
+      <c r="E13">
+        <v>518.5</v>
+      </c>
+      <c r="G13">
+        <v>1942</v>
+      </c>
+      <c r="I13">
+        <v>3.7450000000000001</v>
+      </c>
+      <c r="J13">
+        <v>1198</v>
+      </c>
+      <c r="K13">
+        <v>282.58999999999997</v>
+      </c>
+      <c r="L13">
+        <v>2902</v>
+      </c>
+      <c r="M13" t="s">
+        <v>237</v>
+      </c>
+      <c r="N13" t="s">
+        <v>239</v>
+      </c>
+      <c r="O13" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>255</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>782.1</v>
+      </c>
+      <c r="E14">
+        <v>528.79999999999995</v>
+      </c>
+      <c r="G14">
+        <v>1925</v>
+      </c>
+      <c r="I14">
+        <v>3.6402999999999999</v>
+      </c>
+      <c r="J14">
+        <v>1198</v>
+      </c>
+      <c r="K14">
+        <v>309.07</v>
+      </c>
+      <c r="L14">
+        <v>2847</v>
+      </c>
+      <c r="M14" t="s">
+        <v>237</v>
+      </c>
+      <c r="N14" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>256</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>751.7</v>
+      </c>
+      <c r="E15">
+        <v>522.1</v>
+      </c>
+      <c r="G15">
+        <v>1926</v>
+      </c>
+      <c r="I15">
+        <v>3.6888000000000001</v>
+      </c>
+      <c r="J15">
+        <v>1198</v>
+      </c>
+      <c r="K15">
+        <v>303.2</v>
+      </c>
+      <c r="L15">
+        <v>2773</v>
+      </c>
+      <c r="M15" t="s">
+        <v>237</v>
+      </c>
+      <c r="N15" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>257</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>729.8</v>
+      </c>
+      <c r="E16">
+        <v>501</v>
+      </c>
+      <c r="G16">
+        <v>1879</v>
+      </c>
+      <c r="I16">
+        <v>3.7504</v>
+      </c>
+      <c r="J16">
+        <v>1198</v>
+      </c>
+      <c r="K16">
+        <v>297.8</v>
+      </c>
+      <c r="L16">
+        <v>2737</v>
+      </c>
+      <c r="M16" t="s">
+        <v>237</v>
+      </c>
+      <c r="N16" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>259</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <v>764.9</v>
+      </c>
+      <c r="E18">
+        <v>526.46</v>
+      </c>
+      <c r="G18">
+        <v>351</v>
+      </c>
+      <c r="I18">
+        <v>0.66669999999999996</v>
+      </c>
+      <c r="J18">
+        <v>238</v>
+      </c>
+      <c r="K18">
+        <v>59.28</v>
+      </c>
+      <c r="L18">
+        <v>510</v>
+      </c>
+      <c r="M18" t="s">
+        <v>237</v>
+      </c>
+      <c r="N18" t="s">
+        <v>260</v>
+      </c>
+      <c r="O18" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>261</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>611.15</v>
+      </c>
+      <c r="E19">
+        <v>425.4</v>
+      </c>
+      <c r="G19">
+        <v>316</v>
+      </c>
+      <c r="I19">
+        <v>0.7429</v>
+      </c>
+      <c r="J19">
+        <v>238</v>
+      </c>
+      <c r="K19">
+        <v>47.3</v>
+      </c>
+      <c r="L19">
+        <v>454</v>
+      </c>
+      <c r="M19" t="s">
+        <v>237</v>
+      </c>
+      <c r="N19" t="s">
+        <v>260</v>
+      </c>
+      <c r="O19" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>262</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20">
+        <v>670</v>
+      </c>
+      <c r="E20">
+        <v>440.8</v>
+      </c>
+      <c r="G20">
+        <v>308</v>
+      </c>
+      <c r="I20">
+        <v>0.69869999999999999</v>
+      </c>
+      <c r="J20">
+        <v>238</v>
+      </c>
+      <c r="K20">
+        <v>51.52</v>
+      </c>
+      <c r="L20">
+        <v>487</v>
+      </c>
+      <c r="M20" t="s">
+        <v>237</v>
+      </c>
+      <c r="N20" t="s">
+        <v>260</v>
+      </c>
+      <c r="O20" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>263</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21">
+        <v>703.26</v>
+      </c>
+      <c r="E21">
+        <v>460.6</v>
+      </c>
+      <c r="G21">
+        <v>336</v>
+      </c>
+      <c r="I21">
+        <v>0.72950000000000004</v>
+      </c>
+      <c r="J21">
+        <v>238</v>
+      </c>
+      <c r="K21">
+        <v>62.9</v>
+      </c>
+      <c r="L21">
+        <v>513</v>
+      </c>
+      <c r="M21" t="s">
+        <v>237</v>
+      </c>
+      <c r="N21" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>264</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22">
+        <v>690.6</v>
+      </c>
+      <c r="E22">
+        <v>476.3</v>
+      </c>
+      <c r="G22">
+        <v>320</v>
+      </c>
+      <c r="I22">
+        <v>0.67190000000000005</v>
+      </c>
+      <c r="J22">
+        <v>238</v>
+      </c>
+      <c r="K22">
+        <v>57.8</v>
+      </c>
+      <c r="L22">
+        <v>464</v>
+      </c>
+      <c r="M22" t="s">
+        <v>237</v>
+      </c>
+      <c r="N22" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>265</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23">
+        <v>857.8</v>
+      </c>
+      <c r="E23">
+        <v>481.59</v>
+      </c>
+      <c r="G23">
+        <v>320</v>
+      </c>
+      <c r="I23">
+        <v>0.66449999999999998</v>
+      </c>
+      <c r="J23">
+        <v>238</v>
+      </c>
+      <c r="K23">
+        <v>60.24</v>
+      </c>
+      <c r="L23">
+        <v>570</v>
+      </c>
+      <c r="M23" t="s">
+        <v>237</v>
+      </c>
+      <c r="N23" t="s">
+        <v>266</v>
+      </c>
+      <c r="O23" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>268</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24">
+        <v>692</v>
+      </c>
+      <c r="E24">
+        <v>412.49</v>
+      </c>
+      <c r="G24">
+        <v>304</v>
+      </c>
+      <c r="I24">
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="J24">
+        <v>238</v>
+      </c>
+      <c r="K24">
+        <v>61.08</v>
+      </c>
+      <c r="L24">
+        <v>510</v>
+      </c>
+      <c r="M24" t="s">
+        <v>237</v>
+      </c>
+      <c r="N24" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>269</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25">
+        <v>689</v>
+      </c>
+      <c r="E25">
+        <v>430.7</v>
+      </c>
+      <c r="G25">
+        <v>297</v>
+      </c>
+      <c r="I25">
+        <v>0.68959999999999999</v>
+      </c>
+      <c r="J25">
+        <v>238</v>
+      </c>
+      <c r="K25">
+        <v>59.3</v>
+      </c>
+      <c r="L25">
+        <v>475</v>
+      </c>
+      <c r="M25" t="s">
+        <v>237</v>
+      </c>
+      <c r="N25" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>270</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26">
+        <v>716.3</v>
+      </c>
+      <c r="E26">
+        <v>435.27</v>
+      </c>
+      <c r="G26">
+        <v>302</v>
+      </c>
+      <c r="I26">
+        <v>0.69379999999999997</v>
+      </c>
+      <c r="J26">
+        <v>238</v>
+      </c>
+      <c r="K26">
+        <v>52.6</v>
+      </c>
+      <c r="L26">
+        <v>497</v>
+      </c>
+      <c r="M26" t="s">
+        <v>237</v>
+      </c>
+      <c r="N26" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>271</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27">
+        <v>736.4</v>
+      </c>
+      <c r="E27">
+        <v>418.44</v>
+      </c>
+      <c r="F27">
+        <v>407.9</v>
+      </c>
+      <c r="G27">
+        <v>279</v>
+      </c>
+      <c r="H27">
+        <v>272</v>
+      </c>
+      <c r="I27">
+        <v>0.66679999999999995</v>
+      </c>
+      <c r="J27">
+        <v>238</v>
+      </c>
+      <c r="K27">
+        <v>58.9</v>
+      </c>
+      <c r="L27">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B28" s="2">
+        <v>1</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="2">
+        <v>816.4</v>
+      </c>
+      <c r="E28" s="2">
+        <v>329.1</v>
+      </c>
+      <c r="G28" s="2">
+        <v>212</v>
+      </c>
+      <c r="I28" s="2">
+        <v>0.64429999999999998</v>
+      </c>
+      <c r="J28" s="2">
+        <v>238</v>
+      </c>
+      <c r="K28" s="2">
+        <v>63.6</v>
+      </c>
+      <c r="L28" s="2">
+        <v>526</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>273</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29">
+        <v>793.4</v>
+      </c>
+      <c r="E29">
+        <v>461.1</v>
+      </c>
+      <c r="F29">
+        <v>430.1</v>
+      </c>
+      <c r="G29">
+        <v>297</v>
+      </c>
+      <c r="H29">
+        <v>277</v>
+      </c>
+      <c r="I29">
+        <v>0.64410000000000001</v>
+      </c>
+      <c r="J29">
+        <v>238</v>
+      </c>
+      <c r="K29">
+        <v>63.566000000000003</v>
+      </c>
+      <c r="L29">
+        <v>511</v>
+      </c>
+      <c r="M29" t="s">
+        <v>274</v>
+      </c>
+      <c r="N29" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>277</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30">
+        <v>753.1</v>
+      </c>
+      <c r="E30">
+        <v>432.5</v>
+      </c>
+      <c r="F30">
+        <v>420.4</v>
+      </c>
+      <c r="G30">
+        <v>286</v>
+      </c>
+      <c r="H30">
+        <v>278</v>
+      </c>
+      <c r="I30">
+        <v>0.66120000000000001</v>
+      </c>
+      <c r="J30">
+        <v>238</v>
+      </c>
+      <c r="K30">
+        <v>59</v>
+      </c>
+      <c r="L30">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>279</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31">
+        <v>710.2</v>
+      </c>
+      <c r="E31">
+        <v>419.73</v>
+      </c>
+      <c r="F31">
+        <v>398.9</v>
+      </c>
+      <c r="G31">
+        <v>302</v>
+      </c>
+      <c r="H31">
+        <v>287</v>
+      </c>
+      <c r="I31">
+        <v>0.71950000000000003</v>
+      </c>
+      <c r="J31">
+        <v>238</v>
+      </c>
+      <c r="K31">
+        <v>65.27</v>
+      </c>
+      <c r="L31">
+        <v>511</v>
+      </c>
+      <c r="M31" t="s">
+        <v>280</v>
+      </c>
+      <c r="N31" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>282</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32">
+        <v>775.1</v>
+      </c>
+      <c r="E32">
+        <v>444.89</v>
+      </c>
+      <c r="F32">
+        <v>429.6</v>
+      </c>
+      <c r="G32">
+        <v>291</v>
+      </c>
+      <c r="H32">
+        <v>281</v>
+      </c>
+      <c r="I32">
+        <v>0.65410000000000001</v>
+      </c>
+      <c r="J32">
+        <v>238</v>
+      </c>
+      <c r="K32">
+        <v>61</v>
+      </c>
+      <c r="L32">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>283</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33">
+        <v>752</v>
+      </c>
+      <c r="E33">
+        <v>431</v>
+      </c>
+      <c r="F33">
+        <v>404.25</v>
+      </c>
+      <c r="G33">
+        <v>290</v>
+      </c>
+      <c r="H33">
+        <v>272</v>
+      </c>
+      <c r="I33">
+        <v>0.67290000000000005</v>
+      </c>
+      <c r="J33">
+        <v>238</v>
+      </c>
+      <c r="K33">
+        <v>57.6</v>
+      </c>
+      <c r="L33">
+        <v>506</v>
+      </c>
+      <c r="M33" t="s">
+        <v>284</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
first runs with new debubble cartridge plumbing. but really, first run 1ml vs 5ml horz with refill w/debubble checked. seems to help discrepancy
</commit_message>
<xml_diff>
--- a/Development/IFCB_vehicles/VehicleLabExperimentFiles.xlsx
+++ b/Development/IFCB_vehicles/VehicleLabExperimentFiles.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\from_Samwise\ifcb-analysis\Development\IFCB_vehicles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\ifcb-analysis\Development\IFCB_vehicles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="5085" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="5085" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="VvsHdiffVol_nogood" sheetId="1" r:id="rId1"/>
     <sheet name="9um_beads" sheetId="2" r:id="rId2"/>
-    <sheet name="Guinardia" sheetId="3" r:id="rId3"/>
+    <sheet name="9um_debubcart" sheetId="4" r:id="rId3"/>
+    <sheet name="Guinardia" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="308">
   <si>
     <t>Filename</t>
   </si>
@@ -881,6 +882,75 @@
   </si>
   <si>
     <t>lots of junkat this point</t>
+  </si>
+  <si>
+    <t>D20160114T191511_IFCB102</t>
+  </si>
+  <si>
+    <t>D20160114T185046_IFCB102</t>
+  </si>
+  <si>
+    <t>D20160114T182143_IFCB102</t>
+  </si>
+  <si>
+    <t>D20160114T183615_IFCB102</t>
+  </si>
+  <si>
+    <t>first 1mlVS5ml test after new debubble cartridge feature</t>
+  </si>
+  <si>
+    <t>first horz run, only noral debubble with refill checked</t>
+  </si>
+  <si>
+    <t>1mlVS5ml with refill checked, this will fix discrepancy?</t>
+  </si>
+  <si>
+    <t>significant pause between last sample ending and this one starting, more sheath ran through</t>
+  </si>
+  <si>
+    <t>D20160114T192246_IFCB102</t>
+  </si>
+  <si>
+    <t>D20160114T194629_IFCB102</t>
+  </si>
+  <si>
+    <t>D20160114T195421_IFCB102</t>
+  </si>
+  <si>
+    <t>D20160114T201758_IFCB102</t>
+  </si>
+  <si>
+    <t>D20160114T203409_IFCB102</t>
+  </si>
+  <si>
+    <t>D20160114T202555_IFCB102</t>
+  </si>
+  <si>
+    <t>D20160114T204155_IFCB102</t>
+  </si>
+  <si>
+    <t>D20160114T205009_IFCB102</t>
+  </si>
+  <si>
+    <t>D20160114T205821_IFCB102</t>
+  </si>
+  <si>
+    <t>D20160114T210706_IFCB102</t>
+  </si>
+  <si>
+    <t>D20160114T212312_IFCB102</t>
+  </si>
+  <si>
+    <t>refill after debubble checked</t>
+  </si>
+  <si>
+    <t>hear consistent repeated ticking during refill injection?</t>
+  </si>
+  <si>
+    <t>D20160114T213919_IFCB102</t>
+  </si>
+  <si>
+    <t>D20160114T215520_IFCB102</t>
   </si>
 </sst>
 </file>
@@ -5074,9 +5144,583 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I18" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1">
+        <v>3166</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.47310000000000002</v>
+      </c>
+      <c r="F2" s="1">
+        <v>238</v>
+      </c>
+      <c r="G2" s="1">
+        <v>118.45</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1498</v>
+      </c>
+      <c r="I2" t="s">
+        <v>291</v>
+      </c>
+      <c r="J2" t="s">
+        <v>289</v>
+      </c>
+      <c r="K2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>288</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>3064</v>
+      </c>
+      <c r="E3">
+        <v>0.47649999999999998</v>
+      </c>
+      <c r="F3">
+        <v>238</v>
+      </c>
+      <c r="G3">
+        <v>117.1</v>
+      </c>
+      <c r="H3">
+        <v>1460</v>
+      </c>
+      <c r="I3" t="s">
+        <v>290</v>
+      </c>
+      <c r="J3" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>286</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>2750</v>
+      </c>
+      <c r="E4">
+        <v>2.5943999999999998</v>
+      </c>
+      <c r="F4">
+        <v>1198</v>
+      </c>
+      <c r="G4">
+        <v>565.78</v>
+      </c>
+      <c r="H4">
+        <v>7135</v>
+      </c>
+      <c r="I4" t="s">
+        <v>292</v>
+      </c>
+      <c r="J4" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>2756</v>
+      </c>
+      <c r="E5">
+        <v>0.52059999999999995</v>
+      </c>
+      <c r="F5">
+        <v>238</v>
+      </c>
+      <c r="G5">
+        <v>113</v>
+      </c>
+      <c r="H5">
+        <v>1440</v>
+      </c>
+      <c r="I5" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>293</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>2744.1</v>
+      </c>
+      <c r="E6">
+        <v>2.6208999999999998</v>
+      </c>
+      <c r="F6">
+        <v>1198</v>
+      </c>
+      <c r="G6">
+        <v>568.94000000000005</v>
+      </c>
+      <c r="H6">
+        <v>7192</v>
+      </c>
+      <c r="I6" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>294</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <v>2841</v>
+      </c>
+      <c r="E7">
+        <v>0.4965</v>
+      </c>
+      <c r="F7">
+        <v>238</v>
+      </c>
+      <c r="G7">
+        <v>112.3</v>
+      </c>
+      <c r="H7">
+        <v>2841</v>
+      </c>
+      <c r="I7" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>295</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>2908.66</v>
+      </c>
+      <c r="E8">
+        <v>2.5221</v>
+      </c>
+      <c r="F8">
+        <v>1198</v>
+      </c>
+      <c r="G8">
+        <v>582.70000000000005</v>
+      </c>
+      <c r="H8">
+        <v>7336</v>
+      </c>
+      <c r="I8" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>296</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>2902.5</v>
+      </c>
+      <c r="E9">
+        <v>0.504</v>
+      </c>
+      <c r="F9">
+        <v>238</v>
+      </c>
+      <c r="G9">
+        <v>116.96</v>
+      </c>
+      <c r="H9">
+        <v>1463</v>
+      </c>
+      <c r="I9" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>298</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>3092.88</v>
+      </c>
+      <c r="E10">
+        <v>0.47399999999999998</v>
+      </c>
+      <c r="F10">
+        <v>238</v>
+      </c>
+      <c r="G10">
+        <v>116.87</v>
+      </c>
+      <c r="H10">
+        <v>1466</v>
+      </c>
+      <c r="I10" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>297</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>2990.8</v>
+      </c>
+      <c r="E11">
+        <v>0.48620000000000002</v>
+      </c>
+      <c r="F11">
+        <v>238</v>
+      </c>
+      <c r="G11">
+        <v>114.7</v>
+      </c>
+      <c r="H11">
+        <v>1454</v>
+      </c>
+      <c r="I11" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>299</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <v>3339.4</v>
+      </c>
+      <c r="E12">
+        <v>0.46089999999999998</v>
+      </c>
+      <c r="F12">
+        <v>238</v>
+      </c>
+      <c r="G12">
+        <v>120.9</v>
+      </c>
+      <c r="H12">
+        <v>1539</v>
+      </c>
+      <c r="I12" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>300</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13">
+        <v>3198</v>
+      </c>
+      <c r="E13">
+        <v>0.46870000000000001</v>
+      </c>
+      <c r="F13">
+        <v>238</v>
+      </c>
+      <c r="G13">
+        <v>118.5</v>
+      </c>
+      <c r="H13">
+        <v>1499</v>
+      </c>
+      <c r="I13" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>301</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>3101</v>
+      </c>
+      <c r="E14">
+        <v>0.49370000000000003</v>
+      </c>
+      <c r="F14">
+        <v>238</v>
+      </c>
+      <c r="G14">
+        <v>119.5</v>
+      </c>
+      <c r="H14">
+        <v>1531</v>
+      </c>
+      <c r="I14" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>302</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15">
+        <v>3033.4</v>
+      </c>
+      <c r="E15">
+        <v>1.4851000000000001</v>
+      </c>
+      <c r="F15">
+        <v>718</v>
+      </c>
+      <c r="G15">
+        <v>355</v>
+      </c>
+      <c r="H15">
+        <v>4505</v>
+      </c>
+      <c r="I15" t="s">
+        <v>304</v>
+      </c>
+      <c r="J15" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>303</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>3294</v>
+      </c>
+      <c r="E16">
+        <v>1.4317</v>
+      </c>
+      <c r="F16">
+        <v>718</v>
+      </c>
+      <c r="G16">
+        <v>374.36</v>
+      </c>
+      <c r="H16">
+        <v>4716</v>
+      </c>
+      <c r="I16" t="s">
+        <v>304</v>
+      </c>
+      <c r="J16" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>306</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <v>3109.9</v>
+      </c>
+      <c r="E17">
+        <v>1.4817</v>
+      </c>
+      <c r="F17">
+        <v>718</v>
+      </c>
+      <c r="G17">
+        <v>362.35</v>
+      </c>
+      <c r="H17">
+        <v>4608</v>
+      </c>
+      <c r="I17" t="s">
+        <v>304</v>
+      </c>
+      <c r="J17" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>307</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <v>34.630000000000003</v>
+      </c>
+      <c r="E18">
+        <v>1.3868</v>
+      </c>
+      <c r="F18">
+        <v>718</v>
+      </c>
+      <c r="G18">
+        <v>378.3</v>
+      </c>
+      <c r="H18">
+        <v>4803</v>
+      </c>
+      <c r="I18" t="s">
+        <v>304</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D33" sqref="D33:E33"/>
     </sheetView>

</xml_diff>

<commit_message>
update filenames, don't want IFCB102 in name
</commit_message>
<xml_diff>
--- a/Development/IFCB_vehicles/VehicleLabExperimentFiles.xlsx
+++ b/Development/IFCB_vehicles/VehicleLabExperimentFiles.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\ifcb-analysis\Development\IFCB_vehicles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\from_Samwise\ifcb-analysis\Development\IFCB_vehicles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -884,18 +884,6 @@
     <t>lots of junkat this point</t>
   </si>
   <si>
-    <t>D20160114T191511_IFCB102</t>
-  </si>
-  <si>
-    <t>D20160114T185046_IFCB102</t>
-  </si>
-  <si>
-    <t>D20160114T182143_IFCB102</t>
-  </si>
-  <si>
-    <t>D20160114T183615_IFCB102</t>
-  </si>
-  <si>
     <t>first 1mlVS5ml test after new debubble cartridge feature</t>
   </si>
   <si>
@@ -908,49 +896,61 @@
     <t>significant pause between last sample ending and this one starting, more sheath ran through</t>
   </si>
   <si>
-    <t>D20160114T192246_IFCB102</t>
-  </si>
-  <si>
-    <t>D20160114T194629_IFCB102</t>
-  </si>
-  <si>
-    <t>D20160114T195421_IFCB102</t>
-  </si>
-  <si>
-    <t>D20160114T201758_IFCB102</t>
-  </si>
-  <si>
-    <t>D20160114T203409_IFCB102</t>
-  </si>
-  <si>
-    <t>D20160114T202555_IFCB102</t>
-  </si>
-  <si>
-    <t>D20160114T204155_IFCB102</t>
-  </si>
-  <si>
-    <t>D20160114T205009_IFCB102</t>
-  </si>
-  <si>
-    <t>D20160114T205821_IFCB102</t>
-  </si>
-  <si>
-    <t>D20160114T210706_IFCB102</t>
-  </si>
-  <si>
-    <t>D20160114T212312_IFCB102</t>
-  </si>
-  <si>
     <t>refill after debubble checked</t>
   </si>
   <si>
     <t>hear consistent repeated ticking during refill injection?</t>
   </si>
   <si>
-    <t>D20160114T213919_IFCB102</t>
-  </si>
-  <si>
-    <t>D20160114T215520_IFCB102</t>
+    <t>D20160114T182143</t>
+  </si>
+  <si>
+    <t>D20160114T183615</t>
+  </si>
+  <si>
+    <t>D20160114T185046</t>
+  </si>
+  <si>
+    <t>D20160114T191511</t>
+  </si>
+  <si>
+    <t>D20160114T192246</t>
+  </si>
+  <si>
+    <t>D20160114T194629</t>
+  </si>
+  <si>
+    <t>D20160114T195421</t>
+  </si>
+  <si>
+    <t>D20160114T201758</t>
+  </si>
+  <si>
+    <t>D20160114T202555</t>
+  </si>
+  <si>
+    <t>D20160114T203409</t>
+  </si>
+  <si>
+    <t>D20160114T204155</t>
+  </si>
+  <si>
+    <t>D20160114T205009</t>
+  </si>
+  <si>
+    <t>D20160114T205821</t>
+  </si>
+  <si>
+    <t>D20160114T210706</t>
+  </si>
+  <si>
+    <t>D20160114T212312</t>
+  </si>
+  <si>
+    <t>D20160114T213919</t>
+  </si>
+  <si>
+    <t>D20160114T215520</t>
   </si>
 </sst>
 </file>
@@ -5147,8 +5147,8 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I18" sqref="I18"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5199,7 +5199,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -5223,18 +5223,18 @@
         <v>1498</v>
       </c>
       <c r="I2" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J2" t="s">
+        <v>285</v>
+      </c>
+      <c r="K2" t="s">
         <v>289</v>
-      </c>
-      <c r="K2" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -5258,15 +5258,15 @@
         <v>1460</v>
       </c>
       <c r="I3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="J3" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>286</v>
+        <v>293</v>
       </c>
       <c r="B4">
         <v>5</v>
@@ -5290,15 +5290,15 @@
         <v>7135</v>
       </c>
       <c r="I4" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="J4" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -5322,12 +5322,12 @@
         <v>1440</v>
       </c>
       <c r="I5" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -5351,12 +5351,12 @@
         <v>7192</v>
       </c>
       <c r="I6" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -5380,12 +5380,12 @@
         <v>2841</v>
       </c>
       <c r="I7" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B8">
         <v>5</v>
@@ -5409,12 +5409,12 @@
         <v>7336</v>
       </c>
       <c r="I8" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -5438,12 +5438,12 @@
         <v>1463</v>
       </c>
       <c r="I9" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -5467,12 +5467,12 @@
         <v>1466</v>
       </c>
       <c r="I10" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -5496,12 +5496,12 @@
         <v>1454</v>
       </c>
       <c r="I11" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -5525,12 +5525,12 @@
         <v>1539</v>
       </c>
       <c r="I12" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -5554,12 +5554,12 @@
         <v>1499</v>
       </c>
       <c r="I13" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -5583,12 +5583,12 @@
         <v>1531</v>
       </c>
       <c r="I14" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B15">
         <v>3</v>
@@ -5612,15 +5612,15 @@
         <v>4505</v>
       </c>
       <c r="I15" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
       <c r="J15" t="s">
-        <v>305</v>
+        <v>290</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="B16">
         <v>3</v>
@@ -5644,10 +5644,10 @@
         <v>4716</v>
       </c>
       <c r="I16" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
       <c r="J16" t="s">
-        <v>305</v>
+        <v>290</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -5676,10 +5676,10 @@
         <v>4608</v>
       </c>
       <c r="I17" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
       <c r="J17" t="s">
-        <v>305</v>
+        <v>290</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -5708,7 +5708,7 @@
         <v>4803</v>
       </c>
       <c r="I18" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
     </row>
   </sheetData>

</xml_diff>